<commit_message>
Sliding window: Aditya verma
</commit_message>
<xml_diff>
--- a/StudyPlan.xlsx
+++ b/StudyPlan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rammisra/Documents/GitHub/Learning/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rammi\Documents\Ram\Learning\ram-err404\Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA2621C-8863-344F-820C-77062C3EC13E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0750A7-D796-4609-8DE0-FC0449339BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="3680" windowWidth="37640" windowHeight="21500" xr2:uid="{DBD4FF11-46FB-5146-978E-3349D45A0734}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{DBD4FF11-46FB-5146-978E-3349D45A0734}"/>
   </bookViews>
   <sheets>
     <sheet name="StudyPlan" sheetId="1" r:id="rId1"/>
@@ -29,8 +29,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="102">
   <si>
     <t>Programming Topics</t>
   </si>
@@ -338,13 +336,19 @@
   </si>
   <si>
     <t>10 questions Daily</t>
+  </si>
+  <si>
+    <t>DOne</t>
+  </si>
+  <si>
+    <t>Question</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -402,6 +406,13 @@
     </font>
     <font>
       <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -544,9 +555,6 @@
   </cellStyleXfs>
   <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -564,25 +572,28 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -900,43 +911,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFD5D966-A553-4B41-A091-93A2232C9F0E}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="11" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" style="11" customWidth="1"/>
-    <col min="6" max="6" width="15.1640625" style="12" customWidth="1"/>
-    <col min="7" max="7" width="24.1640625" customWidth="1"/>
-    <col min="8" max="8" width="43.6640625" customWidth="1"/>
-    <col min="9" max="9" width="22.1640625" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="8.625" customWidth="1"/>
+    <col min="2" max="2" width="32.625" customWidth="1"/>
+    <col min="3" max="3" width="18.625" customWidth="1"/>
+    <col min="4" max="4" width="10.625" customWidth="1"/>
+    <col min="5" max="5" width="12.875" customWidth="1"/>
+    <col min="6" max="6" width="15.125" style="10" customWidth="1"/>
+    <col min="7" max="7" width="24.125" customWidth="1"/>
+    <col min="8" max="8" width="43.625" customWidth="1"/>
+    <col min="9" max="9" width="22.125" customWidth="1"/>
+    <col min="10" max="10" width="15.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17" thickBot="1">
-      <c r="A1" s="14"/>
-      <c r="B1" s="15" t="s">
+    <row r="1" spans="1:10" ht="16.5" thickBot="1">
+      <c r="A1" s="12"/>
+      <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="17" t="s">
+      <c r="C1" s="14"/>
+      <c r="D1" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="19"/>
+      <c r="H1" s="16"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
@@ -945,13 +956,16 @@
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="13">
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="11">
         <v>45337</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="11">
         <v>45346</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="10" t="s">
         <v>70</v>
       </c>
       <c r="G2" t="s">
@@ -965,7 +979,10 @@
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="13">
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="11">
         <v>45347</v>
       </c>
       <c r="G3" t="s">
@@ -976,6 +993,9 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
       <c r="G4" t="s">
         <v>7</v>
       </c>
@@ -987,7 +1007,10 @@
       <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="10" t="s">
         <v>71</v>
       </c>
       <c r="G5" t="s">
@@ -998,6 +1021,9 @@
       <c r="B6" t="s">
         <v>10</v>
       </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
       <c r="G6" t="s">
         <v>11</v>
       </c>
@@ -1009,10 +1035,13 @@
       <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="13">
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="11">
         <v>45347</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="10" t="s">
         <v>72</v>
       </c>
       <c r="G7" t="s">
@@ -1023,11 +1052,17 @@
       <c r="B8" t="s">
         <v>14</v>
       </c>
+      <c r="C8" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="9" spans="1:10">
       <c r="B9" t="s">
         <v>15</v>
       </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
@@ -1036,7 +1071,10 @@
       <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="10" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1047,14 +1085,20 @@
       <c r="B11" t="s">
         <v>17</v>
       </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="12" spans="1:10">
       <c r="B12" t="s">
         <v>18</v>
       </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1068,13 +1112,13 @@
       <c r="C15" t="s">
         <v>77</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="11">
         <v>45348</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="H15" s="10" t="s">
+      <c r="H15" s="9" t="s">
         <v>35</v>
       </c>
       <c r="I15" t="s">
@@ -1091,10 +1135,10 @@
       <c r="C16" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="11">
         <v>45348</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="10" t="s">
         <v>72</v>
       </c>
       <c r="H16" t="s">
@@ -1114,10 +1158,13 @@
       <c r="B17" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="13">
+      <c r="C17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="11">
         <v>45347</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="F17" s="10" t="s">
         <v>72</v>
       </c>
       <c r="H17" t="s">
@@ -1134,10 +1181,13 @@
       <c r="B18" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="13">
+      <c r="C18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="11">
         <v>45348</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="F18" s="10" t="s">
         <v>72</v>
       </c>
       <c r="H18" t="s">
@@ -1154,10 +1204,13 @@
       <c r="B19" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="13">
+      <c r="C19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="11">
         <v>45348</v>
       </c>
-      <c r="F19" s="12" t="s">
+      <c r="F19" s="10" t="s">
         <v>72</v>
       </c>
       <c r="H19" t="s">
@@ -1190,6 +1243,9 @@
       <c r="B22" t="s">
         <v>26</v>
       </c>
+      <c r="C22" t="s">
+        <v>39</v>
+      </c>
       <c r="H22" t="s">
         <v>91</v>
       </c>
@@ -1204,7 +1260,7 @@
       <c r="B23" t="s">
         <v>27</v>
       </c>
-      <c r="F23" s="12" t="s">
+      <c r="F23" s="10" t="s">
         <v>73</v>
       </c>
       <c r="H23" t="s">
@@ -1221,7 +1277,7 @@
       <c r="B24" t="s">
         <v>28</v>
       </c>
-      <c r="F24" s="12" t="s">
+      <c r="F24" s="10" t="s">
         <v>73</v>
       </c>
       <c r="H24" t="s">
@@ -1279,6 +1335,9 @@
       <c r="B29" t="s">
         <v>8</v>
       </c>
+      <c r="C29" t="s">
+        <v>39</v>
+      </c>
       <c r="H29" t="s">
         <v>26</v>
       </c>
@@ -1293,7 +1352,10 @@
       <c r="B30" t="s">
         <v>33</v>
       </c>
-      <c r="F30" s="12" t="s">
+      <c r="C30" t="s">
+        <v>39</v>
+      </c>
+      <c r="F30" s="10" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1301,13 +1363,13 @@
       <c r="A31" t="s">
         <v>69</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="17" t="s">
         <v>79</v>
       </c>
       <c r="C31" t="s">
         <v>80</v>
       </c>
-      <c r="F31" s="12" t="s">
+      <c r="F31" s="10" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1321,25 +1383,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{777FF9AE-CAA8-7C48-8B5E-839EF7342066}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" style="21" customWidth="1"/>
-    <col min="2" max="2" width="27" style="21" customWidth="1"/>
-    <col min="3" max="3" width="112.33203125" style="21" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" style="21" customWidth="1"/>
-    <col min="5" max="5" width="21.83203125" style="21" customWidth="1"/>
-    <col min="6" max="6" width="23.5" style="21" customWidth="1"/>
-    <col min="7" max="7" width="21.6640625" style="21" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="21"/>
+    <col min="1" max="1" width="17.625" style="18" customWidth="1"/>
+    <col min="2" max="2" width="10" style="18" customWidth="1"/>
+    <col min="3" max="3" width="52.625" style="18" customWidth="1"/>
+    <col min="4" max="4" width="81.5" style="18" customWidth="1"/>
+    <col min="5" max="5" width="18.75" style="18" customWidth="1"/>
+    <col min="6" max="6" width="19.375" style="18" customWidth="1"/>
+    <col min="7" max="7" width="20.75" style="18" customWidth="1"/>
+    <col min="8" max="8" width="21.625" style="18" customWidth="1"/>
+    <col min="9" max="16384" width="10.875" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26">
+    <row r="1" spans="1:8" ht="26.25">
       <c r="A1" s="22" t="s">
         <v>82</v>
       </c>
@@ -1349,38 +1412,859 @@
       <c r="E1" s="22"/>
       <c r="F1" s="22"/>
       <c r="G1" s="22"/>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="23" t="s">
+      <c r="H1" s="22"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D3" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="E3" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="F3" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="G3" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="G3" s="23"/>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="21" t="s">
-        <v>4</v>
-      </c>
+      <c r="H3" s="19"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="21">
+        <v>45386</v>
+      </c>
+      <c r="C4" s="21"/>
+      <c r="D4"/>
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="B5"/>
+      <c r="C5"/>
+      <c r="D5"/>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="B6"/>
+      <c r="C6"/>
+      <c r="D6"/>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="B11"/>
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="B12"/>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="G14"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16"/>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18"/>
+      <c r="G18"/>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19"/>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="B20"/>
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="E20"/>
+      <c r="F20"/>
+      <c r="G20"/>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="F21"/>
+      <c r="G21"/>
+    </row>
+    <row r="22" spans="2:7">
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
+      <c r="G22"/>
+    </row>
+    <row r="23" spans="2:7">
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
+      <c r="G23"/>
+    </row>
+    <row r="24" spans="2:7">
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
+      <c r="G24"/>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
+      <c r="G25"/>
+    </row>
+    <row r="26" spans="2:7">
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26"/>
+      <c r="F26"/>
+      <c r="G26"/>
+    </row>
+    <row r="27" spans="2:7">
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="E27"/>
+      <c r="F27"/>
+      <c r="G27"/>
+    </row>
+    <row r="28" spans="2:7">
+      <c r="B28"/>
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="E28"/>
+      <c r="F28"/>
+      <c r="G28"/>
+    </row>
+    <row r="29" spans="2:7">
+      <c r="B29"/>
+      <c r="C29"/>
+      <c r="D29"/>
+      <c r="E29"/>
+      <c r="F29"/>
+      <c r="G29"/>
+    </row>
+    <row r="30" spans="2:7">
+      <c r="B30"/>
+      <c r="C30"/>
+      <c r="D30"/>
+      <c r="E30"/>
+      <c r="F30"/>
+      <c r="G30"/>
+    </row>
+    <row r="31" spans="2:7">
+      <c r="B31"/>
+      <c r="C31"/>
+      <c r="D31"/>
+      <c r="E31"/>
+      <c r="F31"/>
+      <c r="G31"/>
+    </row>
+    <row r="32" spans="2:7">
+      <c r="B32"/>
+      <c r="C32"/>
+      <c r="D32"/>
+      <c r="E32"/>
+      <c r="F32"/>
+      <c r="G32"/>
+    </row>
+    <row r="33" spans="2:7">
+      <c r="B33"/>
+      <c r="C33"/>
+      <c r="D33"/>
+      <c r="E33"/>
+      <c r="F33"/>
+      <c r="G33"/>
+    </row>
+    <row r="34" spans="2:7">
+      <c r="B34"/>
+      <c r="C34"/>
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="F34"/>
+      <c r="G34"/>
+    </row>
+    <row r="35" spans="2:7">
+      <c r="B35"/>
+      <c r="C35"/>
+      <c r="D35"/>
+      <c r="E35"/>
+      <c r="F35"/>
+      <c r="G35"/>
+    </row>
+    <row r="36" spans="2:7">
+      <c r="B36"/>
+      <c r="C36"/>
+      <c r="D36"/>
+      <c r="E36"/>
+      <c r="F36"/>
+      <c r="G36"/>
+    </row>
+    <row r="37" spans="2:7">
+      <c r="B37"/>
+      <c r="C37"/>
+      <c r="D37"/>
+      <c r="E37"/>
+      <c r="F37"/>
+      <c r="G37"/>
+    </row>
+    <row r="38" spans="2:7">
+      <c r="B38"/>
+      <c r="C38"/>
+      <c r="D38"/>
+      <c r="E38"/>
+      <c r="F38"/>
+      <c r="G38"/>
+    </row>
+    <row r="39" spans="2:7">
+      <c r="B39"/>
+      <c r="C39"/>
+      <c r="D39"/>
+      <c r="E39"/>
+      <c r="F39"/>
+      <c r="G39"/>
+    </row>
+    <row r="40" spans="2:7">
+      <c r="B40"/>
+      <c r="C40"/>
+      <c r="D40"/>
+      <c r="E40"/>
+      <c r="F40"/>
+      <c r="G40"/>
+    </row>
+    <row r="41" spans="2:7">
+      <c r="B41"/>
+      <c r="C41"/>
+      <c r="D41"/>
+      <c r="E41"/>
+      <c r="F41"/>
+      <c r="G41"/>
+    </row>
+    <row r="42" spans="2:7">
+      <c r="B42"/>
+      <c r="C42"/>
+      <c r="D42"/>
+      <c r="E42"/>
+      <c r="F42"/>
+      <c r="G42"/>
+    </row>
+    <row r="43" spans="2:7">
+      <c r="B43"/>
+      <c r="C43"/>
+      <c r="D43"/>
+      <c r="E43"/>
+      <c r="F43"/>
+      <c r="G43"/>
+    </row>
+    <row r="44" spans="2:7">
+      <c r="B44"/>
+      <c r="C44"/>
+      <c r="D44"/>
+      <c r="E44"/>
+      <c r="F44"/>
+      <c r="G44"/>
+    </row>
+    <row r="45" spans="2:7">
+      <c r="B45"/>
+      <c r="C45"/>
+      <c r="D45"/>
+      <c r="E45"/>
+      <c r="F45"/>
+      <c r="G45"/>
+    </row>
+    <row r="46" spans="2:7">
+      <c r="B46"/>
+      <c r="C46"/>
+      <c r="D46"/>
+      <c r="E46"/>
+      <c r="F46"/>
+      <c r="G46"/>
+    </row>
+    <row r="47" spans="2:7">
+      <c r="B47"/>
+      <c r="C47"/>
+      <c r="D47"/>
+      <c r="E47"/>
+      <c r="F47"/>
+      <c r="G47"/>
+    </row>
+    <row r="48" spans="2:7">
+      <c r="B48"/>
+      <c r="C48"/>
+      <c r="D48"/>
+      <c r="E48"/>
+      <c r="F48"/>
+      <c r="G48"/>
+    </row>
+    <row r="49" spans="2:7">
+      <c r="B49"/>
+      <c r="C49"/>
+      <c r="D49"/>
+      <c r="E49"/>
+      <c r="F49"/>
+      <c r="G49"/>
+    </row>
+    <row r="50" spans="2:7">
+      <c r="B50"/>
+      <c r="C50"/>
+      <c r="D50"/>
+      <c r="E50"/>
+      <c r="F50"/>
+      <c r="G50"/>
+    </row>
+    <row r="51" spans="2:7">
+      <c r="B51"/>
+      <c r="C51"/>
+      <c r="D51"/>
+      <c r="E51"/>
+      <c r="F51"/>
+      <c r="G51"/>
+    </row>
+    <row r="52" spans="2:7">
+      <c r="B52"/>
+      <c r="C52"/>
+      <c r="D52"/>
+      <c r="E52"/>
+      <c r="F52"/>
+      <c r="G52"/>
+    </row>
+    <row r="53" spans="2:7">
+      <c r="B53"/>
+      <c r="C53"/>
+      <c r="D53"/>
+      <c r="E53"/>
+      <c r="F53"/>
+      <c r="G53"/>
+    </row>
+    <row r="54" spans="2:7">
+      <c r="B54"/>
+      <c r="C54"/>
+      <c r="D54"/>
+      <c r="E54"/>
+      <c r="F54"/>
+      <c r="G54"/>
+    </row>
+    <row r="55" spans="2:7">
+      <c r="B55"/>
+      <c r="C55"/>
+      <c r="D55"/>
+      <c r="E55"/>
+      <c r="F55"/>
+      <c r="G55"/>
+    </row>
+    <row r="56" spans="2:7">
+      <c r="B56"/>
+      <c r="C56"/>
+      <c r="D56"/>
+      <c r="E56"/>
+      <c r="F56"/>
+      <c r="G56"/>
+    </row>
+    <row r="57" spans="2:7">
+      <c r="B57"/>
+      <c r="C57"/>
+      <c r="D57"/>
+      <c r="E57"/>
+      <c r="F57"/>
+      <c r="G57"/>
+    </row>
+    <row r="58" spans="2:7">
+      <c r="B58"/>
+      <c r="C58"/>
+      <c r="D58"/>
+      <c r="E58"/>
+      <c r="F58"/>
+      <c r="G58"/>
+    </row>
+    <row r="59" spans="2:7">
+      <c r="B59"/>
+      <c r="C59"/>
+      <c r="D59"/>
+      <c r="E59"/>
+      <c r="F59"/>
+      <c r="G59"/>
+    </row>
+    <row r="60" spans="2:7">
+      <c r="B60"/>
+      <c r="C60"/>
+      <c r="D60"/>
+      <c r="E60"/>
+      <c r="F60"/>
+      <c r="G60"/>
+    </row>
+    <row r="61" spans="2:7">
+      <c r="B61"/>
+      <c r="C61"/>
+      <c r="D61"/>
+      <c r="E61"/>
+      <c r="F61"/>
+      <c r="G61"/>
+    </row>
+    <row r="62" spans="2:7">
+      <c r="B62"/>
+      <c r="C62"/>
+      <c r="D62"/>
+      <c r="E62"/>
+      <c r="F62"/>
+      <c r="G62"/>
+    </row>
+    <row r="63" spans="2:7">
+      <c r="B63"/>
+      <c r="C63"/>
+      <c r="D63"/>
+      <c r="E63"/>
+      <c r="F63"/>
+      <c r="G63"/>
+    </row>
+    <row r="64" spans="2:7">
+      <c r="B64"/>
+      <c r="C64"/>
+      <c r="D64"/>
+      <c r="E64"/>
+      <c r="F64"/>
+      <c r="G64"/>
+    </row>
+    <row r="65" spans="2:7">
+      <c r="B65"/>
+      <c r="C65"/>
+      <c r="D65"/>
+      <c r="E65"/>
+      <c r="F65"/>
+      <c r="G65"/>
+    </row>
+    <row r="66" spans="2:7">
+      <c r="B66"/>
+      <c r="C66"/>
+      <c r="D66"/>
+      <c r="E66"/>
+      <c r="F66"/>
+      <c r="G66"/>
+    </row>
+    <row r="67" spans="2:7">
+      <c r="B67"/>
+      <c r="C67"/>
+      <c r="D67"/>
+      <c r="E67"/>
+      <c r="F67"/>
+      <c r="G67"/>
+    </row>
+    <row r="68" spans="2:7">
+      <c r="B68"/>
+      <c r="C68"/>
+      <c r="D68"/>
+      <c r="E68"/>
+      <c r="F68"/>
+      <c r="G68"/>
+    </row>
+    <row r="69" spans="2:7">
+      <c r="B69"/>
+      <c r="C69"/>
+      <c r="D69"/>
+      <c r="E69"/>
+      <c r="F69"/>
+      <c r="G69"/>
+    </row>
+    <row r="70" spans="2:7">
+      <c r="B70"/>
+      <c r="C70"/>
+      <c r="D70"/>
+      <c r="E70"/>
+      <c r="F70"/>
+      <c r="G70"/>
+    </row>
+    <row r="71" spans="2:7">
+      <c r="B71"/>
+      <c r="C71"/>
+      <c r="D71"/>
+      <c r="E71"/>
+      <c r="F71"/>
+      <c r="G71"/>
+    </row>
+    <row r="72" spans="2:7">
+      <c r="B72"/>
+      <c r="C72"/>
+      <c r="D72"/>
+      <c r="E72"/>
+      <c r="F72"/>
+      <c r="G72"/>
+    </row>
+    <row r="73" spans="2:7">
+      <c r="B73"/>
+      <c r="C73"/>
+      <c r="D73"/>
+      <c r="E73"/>
+      <c r="F73"/>
+      <c r="G73"/>
+    </row>
+    <row r="74" spans="2:7">
+      <c r="B74"/>
+      <c r="C74"/>
+      <c r="D74"/>
+      <c r="E74"/>
+      <c r="F74"/>
+      <c r="G74"/>
+    </row>
+    <row r="75" spans="2:7">
+      <c r="B75"/>
+      <c r="C75"/>
+      <c r="D75"/>
+      <c r="E75"/>
+      <c r="F75"/>
+      <c r="G75"/>
+    </row>
+    <row r="76" spans="2:7">
+      <c r="B76"/>
+      <c r="C76"/>
+      <c r="D76"/>
+      <c r="E76"/>
+      <c r="F76"/>
+      <c r="G76"/>
+    </row>
+    <row r="77" spans="2:7">
+      <c r="B77"/>
+      <c r="C77"/>
+      <c r="D77"/>
+      <c r="E77"/>
+      <c r="F77"/>
+      <c r="G77"/>
+    </row>
+    <row r="78" spans="2:7">
+      <c r="B78"/>
+      <c r="C78"/>
+      <c r="D78"/>
+      <c r="E78"/>
+      <c r="F78"/>
+      <c r="G78"/>
+    </row>
+    <row r="79" spans="2:7">
+      <c r="B79"/>
+      <c r="C79"/>
+      <c r="D79"/>
+      <c r="E79"/>
+      <c r="F79"/>
+      <c r="G79"/>
+    </row>
+    <row r="80" spans="2:7">
+      <c r="B80"/>
+      <c r="C80"/>
+      <c r="D80"/>
+      <c r="E80"/>
+      <c r="F80"/>
+      <c r="G80"/>
+    </row>
+    <row r="81" spans="2:7">
+      <c r="B81"/>
+      <c r="C81"/>
+      <c r="D81"/>
+      <c r="E81"/>
+      <c r="F81"/>
+      <c r="G81"/>
+    </row>
+    <row r="82" spans="2:7">
+      <c r="B82"/>
+      <c r="C82"/>
+      <c r="D82"/>
+      <c r="E82"/>
+      <c r="F82"/>
+      <c r="G82"/>
+    </row>
+    <row r="83" spans="2:7">
+      <c r="B83"/>
+      <c r="C83"/>
+      <c r="D83"/>
+      <c r="E83"/>
+      <c r="F83"/>
+      <c r="G83"/>
+    </row>
+    <row r="84" spans="2:7">
+      <c r="B84"/>
+      <c r="C84"/>
+      <c r="D84"/>
+      <c r="E84"/>
+      <c r="F84"/>
+      <c r="G84"/>
+    </row>
+    <row r="85" spans="2:7">
+      <c r="B85"/>
+      <c r="C85"/>
+      <c r="D85"/>
+      <c r="E85"/>
+      <c r="F85"/>
+      <c r="G85"/>
+    </row>
+    <row r="86" spans="2:7">
+      <c r="B86"/>
+      <c r="C86"/>
+      <c r="D86"/>
+      <c r="E86"/>
+      <c r="F86"/>
+      <c r="G86"/>
+    </row>
+    <row r="87" spans="2:7">
+      <c r="B87"/>
+      <c r="C87"/>
+      <c r="D87"/>
+      <c r="E87"/>
+      <c r="F87"/>
+      <c r="G87"/>
+    </row>
+    <row r="88" spans="2:7">
+      <c r="B88"/>
+      <c r="C88"/>
+      <c r="D88"/>
+      <c r="E88"/>
+      <c r="F88"/>
+      <c r="G88"/>
+    </row>
+    <row r="89" spans="2:7">
+      <c r="B89"/>
+      <c r="C89"/>
+      <c r="D89"/>
+      <c r="E89"/>
+      <c r="F89"/>
+      <c r="G89"/>
+    </row>
+    <row r="90" spans="2:7">
+      <c r="B90"/>
+      <c r="C90"/>
+      <c r="D90"/>
+      <c r="E90"/>
+      <c r="F90"/>
+      <c r="G90"/>
+    </row>
+    <row r="91" spans="2:7">
+      <c r="B91"/>
+      <c r="C91"/>
+      <c r="D91"/>
+      <c r="E91"/>
+      <c r="F91"/>
+      <c r="G91"/>
+    </row>
+    <row r="92" spans="2:7">
+      <c r="B92"/>
+      <c r="C92"/>
+      <c r="D92"/>
+      <c r="E92"/>
+      <c r="F92"/>
+      <c r="G92"/>
+    </row>
+    <row r="93" spans="2:7">
+      <c r="B93"/>
+      <c r="C93"/>
+      <c r="D93"/>
+      <c r="E93"/>
+      <c r="F93"/>
+      <c r="G93"/>
+    </row>
+    <row r="94" spans="2:7">
+      <c r="B94"/>
+      <c r="C94"/>
+      <c r="D94"/>
+      <c r="E94"/>
+      <c r="F94"/>
+      <c r="G94"/>
+    </row>
+    <row r="95" spans="2:7">
+      <c r="B95"/>
+      <c r="C95"/>
+      <c r="D95"/>
+      <c r="E95"/>
+      <c r="F95"/>
+      <c r="G95"/>
+    </row>
+    <row r="96" spans="2:7">
+      <c r="B96"/>
+      <c r="C96"/>
+      <c r="D96"/>
+      <c r="E96"/>
+      <c r="F96"/>
+      <c r="G96"/>
+    </row>
+    <row r="97" spans="2:7">
+      <c r="B97"/>
+      <c r="C97"/>
+      <c r="D97"/>
+      <c r="E97"/>
+      <c r="F97"/>
+      <c r="G97"/>
+    </row>
+    <row r="98" spans="2:7">
+      <c r="B98"/>
+      <c r="C98"/>
+      <c r="D98"/>
+      <c r="E98"/>
+      <c r="F98"/>
+      <c r="G98"/>
+    </row>
+    <row r="99" spans="2:7">
+      <c r="B99"/>
+      <c r="C99"/>
+      <c r="D99"/>
+      <c r="E99"/>
+      <c r="F99"/>
+      <c r="G99"/>
+    </row>
+    <row r="100" spans="2:7">
+      <c r="B100"/>
+      <c r="C100"/>
+      <c r="D100"/>
+      <c r="E100"/>
+      <c r="F100"/>
+      <c r="G100"/>
+    </row>
+    <row r="101" spans="2:7">
+      <c r="B101"/>
+      <c r="C101"/>
+      <c r="D101"/>
+      <c r="E101"/>
+      <c r="F101"/>
+      <c r="G101"/>
+    </row>
+    <row r="102" spans="2:7">
+      <c r="B102"/>
+      <c r="C102"/>
+      <c r="D102"/>
+      <c r="E102"/>
+      <c r="F102"/>
+      <c r="G102"/>
+    </row>
+    <row r="103" spans="2:7">
+      <c r="B103"/>
+      <c r="C103"/>
+      <c r="D103"/>
+      <c r="E103"/>
+      <c r="F103"/>
+      <c r="G103"/>
+    </row>
+    <row r="104" spans="2:7">
+      <c r="B104"/>
+      <c r="C104"/>
+      <c r="D104"/>
+      <c r="E104"/>
+      <c r="F104"/>
+      <c r="G104"/>
+    </row>
+    <row r="105" spans="2:7">
+      <c r="B105"/>
+      <c r="C105"/>
+      <c r="D105"/>
+      <c r="E105"/>
+      <c r="F105"/>
+      <c r="G105"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1392,34 +2276,34 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" customWidth="1"/>
-    <col min="2" max="2" width="56.33203125" customWidth="1"/>
-    <col min="3" max="3" width="35.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.125" customWidth="1"/>
+    <col min="2" max="2" width="56.375" customWidth="1"/>
+    <col min="3" max="3" width="35.625" customWidth="1"/>
     <col min="4" max="4" width="19.5" customWidth="1"/>
-    <col min="5" max="5" width="49.6640625" customWidth="1"/>
+    <col min="5" max="5" width="49.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="17" thickBot="1">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="2:5" ht="16.5" thickBot="1">
+      <c r="B2" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="2:5" ht="18" thickTop="1" thickBot="1">
-      <c r="B3" s="2" t="s">
+      <c r="C2" s="23"/>
+    </row>
+    <row r="3" spans="2:5" ht="17.25" thickTop="1" thickBot="1">
+      <c r="B3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="17" thickTop="1">
-      <c r="B4" s="3" t="s">
+    <row r="4" spans="2:5" ht="16.5" thickTop="1">
+      <c r="B4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D4" t="s">
@@ -1430,10 +2314,10 @@
       </c>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D5" t="s">
@@ -1444,10 +2328,10 @@
       </c>
     </row>
     <row r="6" spans="2:5">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D6" t="s">
@@ -1455,10 +2339,10 @@
       </c>
     </row>
     <row r="7" spans="2:5">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>45</v>
       </c>
       <c r="D7" t="s">
@@ -1469,10 +2353,10 @@
       </c>
     </row>
     <row r="8" spans="2:5">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>47</v>
       </c>
       <c r="D8" t="s">
@@ -1480,32 +2364,32 @@
       </c>
     </row>
     <row r="9" spans="2:5">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="10" spans="2:5">
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="11" spans="2:5">
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>54</v>
       </c>
       <c r="D11" t="s">
@@ -1513,10 +2397,10 @@
       </c>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>57</v>
       </c>
       <c r="D12" t="s">
@@ -1527,42 +2411,42 @@
       </c>
     </row>
     <row r="13" spans="2:5">
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="14" spans="2:5">
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="15" spans="2:5">
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="16" spans="2:5">
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="17" spans="2:3">
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="8" t="s">
         <v>66</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Algorithms Topics to StudyPlan.xlsx
</commit_message>
<xml_diff>
--- a/StudyPlan.xlsx
+++ b/StudyPlan.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rammi\Documents\Ram\Learning\ram-err404\Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0750A7-D796-4609-8DE0-FC0449339BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E9A80F3-2853-4C1F-AD2C-CAF8A3851238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{DBD4FF11-46FB-5146-978E-3349D45A0734}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{DBD4FF11-46FB-5146-978E-3349D45A0734}"/>
   </bookViews>
   <sheets>
     <sheet name="StudyPlan" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="376">
   <si>
     <t>Programming Topics</t>
   </si>
@@ -342,6 +343,828 @@
   </si>
   <si>
     <t>Question</t>
+  </si>
+  <si>
+    <t>ALGORITHM</t>
+  </si>
+  <si>
+    <t>Traversal: Inorder, Preorder, Postorder</t>
+  </si>
+  <si>
+    <t>BFS: (Shortest Path in matrices)</t>
+  </si>
+  <si>
+    <t>DFS (Traversal, Cycle Detection)</t>
+  </si>
+  <si>
+    <t>Bipartite Graph: (BFS/DFS)</t>
+  </si>
+  <si>
+    <t>Detect Cycle in Directed Graph: DFS</t>
+  </si>
+  <si>
+    <t>Topological Sort: (DFS)</t>
+  </si>
+  <si>
+    <t>Kahn's Algorithm: Topological Sort (Using BFS)</t>
+  </si>
+  <si>
+    <t>Shortest Path in Directed Acyclic Graph: (Topological Sort)</t>
+  </si>
+  <si>
+    <t>Shortest Path in Undirected Graph with unit weights</t>
+  </si>
+  <si>
+    <t>Dijkstra's Algorithm: (Using PQ)</t>
+  </si>
+  <si>
+    <t>Dijkstra's Algorithm: (Using Set)</t>
+  </si>
+  <si>
+    <t>Bellman Ford Algorithm: (Shortest path from all nodes)</t>
+  </si>
+  <si>
+    <t>Floyd Warshall Algorithm</t>
+  </si>
+  <si>
+    <t>Topo Sort</t>
+  </si>
+  <si>
+    <t>Shortest Path</t>
+  </si>
+  <si>
+    <t>Minimum Spanning Tree</t>
+  </si>
+  <si>
+    <t>Prim's Algorithm</t>
+  </si>
+  <si>
+    <t>Disjoint Set Union</t>
+  </si>
+  <si>
+    <t>Kruskal's Algorithm: (Min Spanning Tree using DSU)</t>
+  </si>
+  <si>
+    <t>Strongly Connected Components</t>
+  </si>
+  <si>
+    <t>Kosaraju's Algorithm</t>
+  </si>
+  <si>
+    <t>Bridges in Graph</t>
+  </si>
+  <si>
+    <t>Tarjan's Algorithm: (Time of insertion/lowest time of insertion)</t>
+  </si>
+  <si>
+    <t>Articulation Point in Graph</t>
+  </si>
+  <si>
+    <t>Recursion</t>
+  </si>
+  <si>
+    <t>Merge Sort</t>
+  </si>
+  <si>
+    <t>Quick Sort</t>
+  </si>
+  <si>
+    <t>Subsequences</t>
+  </si>
+  <si>
+    <t>Subsets / Subset sum</t>
+  </si>
+  <si>
+    <t>Combinational Sum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Palindrome Partitioning </t>
+  </si>
+  <si>
+    <t>Count Inversion</t>
+  </si>
+  <si>
+    <t>BackTracking</t>
+  </si>
+  <si>
+    <t>N Queen</t>
+  </si>
+  <si>
+    <t>Sudoko Solver</t>
+  </si>
+  <si>
+    <t>M-Coloring Problem</t>
+  </si>
+  <si>
+    <t>Rat in Maze</t>
+  </si>
+  <si>
+    <t>kth Permutation Sequence</t>
+  </si>
+  <si>
+    <t>Permutation of string</t>
+  </si>
+  <si>
+    <t>Largest Number in k swaps</t>
+  </si>
+  <si>
+    <t>N Digit Numbers with digits in increasing order</t>
+  </si>
+  <si>
+    <t>0/1 Knapsack</t>
+  </si>
+  <si>
+    <t>Subset Sum</t>
+  </si>
+  <si>
+    <t>Equal Sum Partition</t>
+  </si>
+  <si>
+    <t>Count of subsets sum with a given sum</t>
+  </si>
+  <si>
+    <t>Minimum subset sum difference</t>
+  </si>
+  <si>
+    <t>Count the number of subset with a given difference</t>
+  </si>
+  <si>
+    <t>Target Sum</t>
+  </si>
+  <si>
+    <t>Unbounded Knapsack</t>
+  </si>
+  <si>
+    <t>Rod Cutting Problem</t>
+  </si>
+  <si>
+    <t>Coin change problem: Maximum Number of Ways</t>
+  </si>
+  <si>
+    <t>Coin change problem: Minimum Number of coins</t>
+  </si>
+  <si>
+    <t>Longest Common Subsequence</t>
+  </si>
+  <si>
+    <t>Longest Common Substring</t>
+  </si>
+  <si>
+    <t>Prints as well</t>
+  </si>
+  <si>
+    <t>Shortest Common SuperSequence</t>
+  </si>
+  <si>
+    <t>Min # of insertion/deletion to convert String s1 to s2</t>
+  </si>
+  <si>
+    <t>Longest Palindromic Subsequence</t>
+  </si>
+  <si>
+    <t>Min # of deletion in a string to make it a palindrome</t>
+  </si>
+  <si>
+    <t>Longest repeating subsequence</t>
+  </si>
+  <si>
+    <t>Sequence pattern matching</t>
+  </si>
+  <si>
+    <t>Min # of insertion in a string to make it a palindrome</t>
+  </si>
+  <si>
+    <t>Matrix Chain Multiplication (MCM) / Partition DP</t>
+  </si>
+  <si>
+    <t>Matrix Chain Multiplication</t>
+  </si>
+  <si>
+    <t>Palindrome Partitioning</t>
+  </si>
+  <si>
+    <t>Evaluate Expression to True Paranthesization</t>
+  </si>
+  <si>
+    <t>Scrambled String</t>
+  </si>
+  <si>
+    <t>Egg Dropping Problem</t>
+  </si>
+  <si>
+    <t>DP on Trees</t>
+  </si>
+  <si>
+    <t>Diameter of a Binary Tree</t>
+  </si>
+  <si>
+    <t>Max Path Sum | From any node to any node</t>
+  </si>
+  <si>
+    <t>Max Path Sum | From leaf node to leaf node</t>
+  </si>
+  <si>
+    <t>Dynamic Programming (ADITYA VERMA)</t>
+  </si>
+  <si>
+    <t>DP (Striver)</t>
+  </si>
+  <si>
+    <t>Frog Jump</t>
+  </si>
+  <si>
+    <t>House Robber 2</t>
+  </si>
+  <si>
+    <t>Ninja's Training</t>
+  </si>
+  <si>
+    <t>DP on Grid</t>
+  </si>
+  <si>
+    <t>Grid Unique Paths</t>
+  </si>
+  <si>
+    <t>Minimum Path Sum in Grid</t>
+  </si>
+  <si>
+    <t>Min/Max Falling Path Sum</t>
+  </si>
+  <si>
+    <t>Triangle | Fixed starting point and variable ending point</t>
+  </si>
+  <si>
+    <t>Cherry Pickup 2 | (3D DP)</t>
+  </si>
+  <si>
+    <t>Subsequence</t>
+  </si>
+  <si>
+    <t>Subset Sum Equals to Target</t>
+  </si>
+  <si>
+    <t>Coin change 2</t>
+  </si>
+  <si>
+    <t>Rod cutting</t>
+  </si>
+  <si>
+    <t>DP on String</t>
+  </si>
+  <si>
+    <t>Shortest Common Supersequence</t>
+  </si>
+  <si>
+    <t>Distinct subsequences</t>
+  </si>
+  <si>
+    <t>Edit Distance</t>
+  </si>
+  <si>
+    <t>Wildcard Matching</t>
+  </si>
+  <si>
+    <t>DP on Stocks</t>
+  </si>
+  <si>
+    <t>Best Time to buy and sell stocks</t>
+  </si>
+  <si>
+    <t>Buy and Sell Stocks 2</t>
+  </si>
+  <si>
+    <t>Buy and Sell Stocks 3</t>
+  </si>
+  <si>
+    <t>Longest Increasing Subsequences</t>
+  </si>
+  <si>
+    <t>Print LIS</t>
+  </si>
+  <si>
+    <t>Longest Increasing Subsequences | Using Binary Search</t>
+  </si>
+  <si>
+    <t>Count Number of LIS</t>
+  </si>
+  <si>
+    <t>MCM | Partition DP</t>
+  </si>
+  <si>
+    <t>Burst Balloons</t>
+  </si>
+  <si>
+    <t>Evaluate Boolean Expression to True</t>
+  </si>
+  <si>
+    <t>Min cost to cut the strick</t>
+  </si>
+  <si>
+    <t>Partition Array for maximum sum</t>
+  </si>
+  <si>
+    <t>Maximum Rectangle Area with all 1's</t>
+  </si>
+  <si>
+    <t>Count Square submatrices with all 1's</t>
+  </si>
+  <si>
+    <t>Max points you can obtain from cards</t>
+  </si>
+  <si>
+    <t>Longest substring without repeating chars</t>
+  </si>
+  <si>
+    <t>Max Consecutive Ones 3</t>
+  </si>
+  <si>
+    <t>Fruit into Baskets</t>
+  </si>
+  <si>
+    <t>Longest substring with atmost k distinct chars</t>
+  </si>
+  <si>
+    <t>Number of substrings containing all 3 characters</t>
+  </si>
+  <si>
+    <t>Longest Repeating Character replacement</t>
+  </si>
+  <si>
+    <t>Binary Subarray with K different integers</t>
+  </si>
+  <si>
+    <t>Minimum window substring</t>
+  </si>
+  <si>
+    <t>First Negative in every window of size k</t>
+  </si>
+  <si>
+    <t>Count occurences of Anagrams</t>
+  </si>
+  <si>
+    <t>Maximum of all subarrays of size k</t>
+  </si>
+  <si>
+    <t>Largest Subarray of sum k</t>
+  </si>
+  <si>
+    <t>Variable size window</t>
+  </si>
+  <si>
+    <t>Fixed size window</t>
+  </si>
+  <si>
+    <t>ADITYA VERMA</t>
+  </si>
+  <si>
+    <t>Longest substring with k unique chars</t>
+  </si>
+  <si>
+    <t>Pick Toys</t>
+  </si>
+  <si>
+    <t>Binary Search</t>
+  </si>
+  <si>
+    <t>Lower Bound and Upper Bound</t>
+  </si>
+  <si>
+    <t>First and last occurences in Array (Using Lower/Upper Bound)</t>
+  </si>
+  <si>
+    <t>Search in rotated sorted array 2</t>
+  </si>
+  <si>
+    <t>Minimum in rotated sorted array</t>
+  </si>
+  <si>
+    <t>Find out how many times array is rotated</t>
+  </si>
+  <si>
+    <t>Search in matrix (Both rows and cols are sorted)</t>
+  </si>
+  <si>
+    <t>Single element in sorted array</t>
+  </si>
+  <si>
+    <t>Find Peak Element</t>
+  </si>
+  <si>
+    <t>Square root using Binary search</t>
+  </si>
+  <si>
+    <t>Nth root of an interger</t>
+  </si>
+  <si>
+    <t>Koko eating Banana's</t>
+  </si>
+  <si>
+    <t>Minimum days to make M bouquets</t>
+  </si>
+  <si>
+    <t>Smallest divisor for threshold</t>
+  </si>
+  <si>
+    <t>Capacity to ship packages within D Day</t>
+  </si>
+  <si>
+    <t>Kth Missing positive number</t>
+  </si>
+  <si>
+    <t>Aggressive Cows</t>
+  </si>
+  <si>
+    <t>Allocate Books (Google)</t>
+  </si>
+  <si>
+    <t>Painter Partition and Split Array - Largest Sum</t>
+  </si>
+  <si>
+    <t>Minimize Maximum distance between Gas Stations</t>
+  </si>
+  <si>
+    <t>Meadian of 2 Sorted Arrays of Different Sizes</t>
+  </si>
+  <si>
+    <t>Kth element of 2 sorted arrays</t>
+  </si>
+  <si>
+    <t>Row with maximum number of 1's</t>
+  </si>
+  <si>
+    <t>LeetCode Links</t>
+  </si>
+  <si>
+    <t>Add 2 Numbers in LL</t>
+  </si>
+  <si>
+    <t>Odd Even Linked List</t>
+  </si>
+  <si>
+    <t>Sort a LL of 0's, 1's and 2's</t>
+  </si>
+  <si>
+    <t>Remove the nth Node from the end of the LL</t>
+  </si>
+  <si>
+    <t>Reverse a LL/DLL</t>
+  </si>
+  <si>
+    <t>Check if LL is palindrome</t>
+  </si>
+  <si>
+    <t>Find the intersection point of Y LL</t>
+  </si>
+  <si>
+    <t>Find Middle of LL</t>
+  </si>
+  <si>
+    <t>Detect a loop or cycle in LL</t>
+  </si>
+  <si>
+    <t>Find the length of the loop in LL</t>
+  </si>
+  <si>
+    <t>Find the starting point of cycle in LL. (Tortoise and Hare Algorithm)</t>
+  </si>
+  <si>
+    <t>Delete all occurrence of a key in DLL</t>
+  </si>
+  <si>
+    <t>Find all pairs with given Sum in DLL</t>
+  </si>
+  <si>
+    <t>Remove Duplicates from DLL</t>
+  </si>
+  <si>
+    <t>Reverse nodes in K Group Size of LL</t>
+  </si>
+  <si>
+    <t>Rotate a LL</t>
+  </si>
+  <si>
+    <t>Merge 2 Sorted LL</t>
+  </si>
+  <si>
+    <t>Flattening a LL</t>
+  </si>
+  <si>
+    <t>Merge K sorted LL</t>
+  </si>
+  <si>
+    <t>Sort a LL</t>
+  </si>
+  <si>
+    <t>Clone a LL with Next and random pointer</t>
+  </si>
+  <si>
+    <t>Design a Browser History</t>
+  </si>
+  <si>
+    <t>Least Recently Used (LRU) Cache</t>
+  </si>
+  <si>
+    <t>DLL</t>
+  </si>
+  <si>
+    <t>Trees / Binary Trees / Binary Search Trees</t>
+  </si>
+  <si>
+    <t>Traversal</t>
+  </si>
+  <si>
+    <t>Inorder/Preorder/Postorder</t>
+  </si>
+  <si>
+    <t>DFS/BFS (Level Order Traversal)</t>
+  </si>
+  <si>
+    <t>Top View</t>
+  </si>
+  <si>
+    <t>View Specific</t>
+  </si>
+  <si>
+    <t>Max Depth of Tree (Height)</t>
+  </si>
+  <si>
+    <t>Diameter of the Binary Tree</t>
+  </si>
+  <si>
+    <t>Check for Balanced Binary Tree</t>
+  </si>
+  <si>
+    <t>Max Path Sum in Binary Tree</t>
+  </si>
+  <si>
+    <t>Check if 2 Trees are identical or not</t>
+  </si>
+  <si>
+    <t>Zig-Zag or Spiral traversal in Binary Tree</t>
+  </si>
+  <si>
+    <t>Boundary Traversal</t>
+  </si>
+  <si>
+    <t>Vertical Order Traversal</t>
+  </si>
+  <si>
+    <t>Bottom View</t>
+  </si>
+  <si>
+    <t>Right/Left View</t>
+  </si>
+  <si>
+    <t>Check for Symmetrical Binary Trees</t>
+  </si>
+  <si>
+    <t>Lowest Common Ancestor in Binary Tree</t>
+  </si>
+  <si>
+    <t>Maximum Width of Binary Tree</t>
+  </si>
+  <si>
+    <t>Children Sum Property in Binary Tree</t>
+  </si>
+  <si>
+    <t>Minimum Time taken to burn the Binary Tree from a node</t>
+  </si>
+  <si>
+    <t>Create a Unique Binary Tree</t>
+  </si>
+  <si>
+    <t>Construct a Binary Tree from Preorder and Inorder</t>
+  </si>
+  <si>
+    <t>Construct a Binary Tree from Postorder and Inorder</t>
+  </si>
+  <si>
+    <t>Serialize and De-serialize Binary Tree</t>
+  </si>
+  <si>
+    <t>(Imp)</t>
+  </si>
+  <si>
+    <t>Morris Traversal | Preorder | Inorder</t>
+  </si>
+  <si>
+    <t>Flatten a Binary Tree to Linked List</t>
+  </si>
+  <si>
+    <t>Ceil in a Binary Search Tree</t>
+  </si>
+  <si>
+    <t>Floor in a BST</t>
+  </si>
+  <si>
+    <t>Insert in BST</t>
+  </si>
+  <si>
+    <t>Delete in BST</t>
+  </si>
+  <si>
+    <t>Kth Smallest/Largest Element in BST</t>
+  </si>
+  <si>
+    <t>Check if a Tree is BST or BT</t>
+  </si>
+  <si>
+    <t>Construct a BST from preorder</t>
+  </si>
+  <si>
+    <t>Inorder successor/predecessor</t>
+  </si>
+  <si>
+    <t>Two Sum in BST</t>
+  </si>
+  <si>
+    <t>Recover BST</t>
+  </si>
+  <si>
+    <t>Largest BST in Binary Tree</t>
+  </si>
+  <si>
+    <t>Stack and Queues</t>
+  </si>
+  <si>
+    <t>Queue Implementation using Arrays</t>
+  </si>
+  <si>
+    <t>Stack Implementation using a Single Queue</t>
+  </si>
+  <si>
+    <t>Implement Queue using stack | O(1) Push &amp; Pop</t>
+  </si>
+  <si>
+    <t>Valid Parentheses</t>
+  </si>
+  <si>
+    <t>Next Greater Element</t>
+  </si>
+  <si>
+    <t>Implement LRU</t>
+  </si>
+  <si>
+    <t>Implement LFU</t>
+  </si>
+  <si>
+    <t>Largest Rectangle in Histogram</t>
+  </si>
+  <si>
+    <t>Insert | Search | Starts with</t>
+  </si>
+  <si>
+    <t>Insert | countWordsEqualTo()</t>
+  </si>
+  <si>
+    <t>Longest Word with All Prefixes</t>
+  </si>
+  <si>
+    <t>Number of Distinct Substring in a String</t>
+  </si>
+  <si>
+    <t>Bit PreRequisites for Trie problems</t>
+  </si>
+  <si>
+    <t>Maximum XOR of 2 Numbers in an Array</t>
+  </si>
+  <si>
+    <t>Maximum XOR with an Element From Array</t>
+  </si>
+  <si>
+    <t>Greedy Algorithm</t>
+  </si>
+  <si>
+    <t>N meetings in 1 room</t>
+  </si>
+  <si>
+    <t>Minimum Platforms</t>
+  </si>
+  <si>
+    <t>Job Sequencing Problem</t>
+  </si>
+  <si>
+    <t>Fractional Knapsack</t>
+  </si>
+  <si>
+    <t>Minimum Coins</t>
+  </si>
+  <si>
+    <t>2 Pointers</t>
+  </si>
+  <si>
+    <t>3 Sum</t>
+  </si>
+  <si>
+    <t>Trapping Rainwater</t>
+  </si>
+  <si>
+    <t>Remove Duplicates from Sorted Array</t>
+  </si>
+  <si>
+    <t>Max Consecutive Ones</t>
+  </si>
+  <si>
+    <t>4 Sum</t>
+  </si>
+  <si>
+    <t>Reverse Pairs</t>
+  </si>
+  <si>
+    <t>Hashing</t>
+  </si>
+  <si>
+    <t>2 Sum Problem</t>
+  </si>
+  <si>
+    <t>Longest Consecutive Sequence</t>
+  </si>
+  <si>
+    <t>Largest Subarray with Sum</t>
+  </si>
+  <si>
+    <t>Count Subarrays with Xor as K</t>
+  </si>
+  <si>
+    <t>Longest Substring without Repeating Characters</t>
+  </si>
+  <si>
+    <t>Equal Average Partition</t>
+  </si>
+  <si>
+    <t>Advanced Data Structure and Algorithms</t>
+  </si>
+  <si>
+    <t>Fenwick Tree</t>
+  </si>
+  <si>
+    <t>Binary Lifting on Fenwick Tree</t>
+  </si>
+  <si>
+    <t>Segment Tree</t>
+  </si>
+  <si>
+    <t>Lazy Propagation in Segment Tree</t>
+  </si>
+  <si>
+    <t>Multiset (NLogN approach) | Binary Search + Fenwick Tree</t>
+  </si>
+  <si>
+    <t>1's and 2's Compliment</t>
+  </si>
+  <si>
+    <t>Some Tricks:</t>
+  </si>
+  <si>
+    <t>Swap 2 Numbers | Extract/Set/Toggle ith Bit | Count the set bits | Check if power of 2</t>
+  </si>
+  <si>
+    <t>Minimum bit flips to convert number</t>
+  </si>
+  <si>
+    <t>Power Set</t>
+  </si>
+  <si>
+    <t>Single Number - II</t>
+  </si>
+  <si>
+    <t>Single Number - I</t>
+  </si>
+  <si>
+    <t>Single Number - III</t>
+  </si>
+  <si>
+    <t>XOR of Numbers in a given range</t>
+  </si>
+  <si>
+    <t>Divide 2 numbers with division operators</t>
+  </si>
+  <si>
+    <t>Maths PlayList</t>
+  </si>
+  <si>
+    <t>Euclidean Algorithm</t>
+  </si>
+  <si>
+    <t>Print all Divisors of a number</t>
+  </si>
+  <si>
+    <t>Check if a number is Prime or not</t>
+  </si>
+  <si>
+    <t>Print all prime factor of a number</t>
+  </si>
+  <si>
+    <t>Power Exponentiation</t>
+  </si>
+  <si>
+    <t>Sieve of Eratosthenes</t>
+  </si>
+  <si>
+    <t>Count prime in a range L-R</t>
+  </si>
+  <si>
+    <t>Smallest Prime Factor (SPF)</t>
   </si>
 </sst>
 </file>
@@ -1385,7 +2208,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{777FF9AE-CAA8-7C48-8B5E-839EF7342066}">
   <dimension ref="A1:H105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -2464,4 +3287,1411 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32B7A177-E1B8-4ED4-BA59-45DADAF01CAD}">
+  <dimension ref="A1:C301"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A278" workbookViewId="0">
+      <selection activeCell="B295" sqref="B295"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="41" customWidth="1"/>
+    <col min="2" max="2" width="71.5" customWidth="1"/>
+    <col min="3" max="3" width="72.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="B5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="B6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="B8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="B9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="B12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>118</v>
+      </c>
+      <c r="B17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B18" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>122</v>
+      </c>
+      <c r="B20" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>124</v>
+      </c>
+      <c r="B22" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="B23" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="B26" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="B27" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="B28" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="B29" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="B30" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="B31" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="B32" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="B33" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="B34" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="B35" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="B36" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="B37" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="B38" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="B39" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="B40" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>144</v>
+      </c>
+      <c r="B43" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="B44" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="B45" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="B46" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="B47" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="B48" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>151</v>
+      </c>
+      <c r="B50" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="B51" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="B52" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>155</v>
+      </c>
+      <c r="B54" t="s">
+        <v>156</v>
+      </c>
+      <c r="C54" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="B55" t="s">
+        <v>158</v>
+      </c>
+      <c r="C55" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="B56" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="B57" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="B58" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="B59" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="B60" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="B61" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>165</v>
+      </c>
+      <c r="B63" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="B64" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="B65" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="B66" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="B67" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
+        <v>171</v>
+      </c>
+      <c r="B69" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="B70" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="B71" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="9" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="B74" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="B75" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="B76" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
+        <v>180</v>
+      </c>
+      <c r="B78" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="B79" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="B80" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="B81" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="B82" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" t="s">
+        <v>186</v>
+      </c>
+      <c r="B84" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="B85" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="B86" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" t="s">
+        <v>190</v>
+      </c>
+      <c r="B88" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="B89" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="B90" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="B91" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="B92" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="B93" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="B94" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="B97" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="B98" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="B99" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" t="s">
+        <v>199</v>
+      </c>
+      <c r="B101" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="B102" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="B103" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="B104" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" t="s">
+        <v>203</v>
+      </c>
+      <c r="B106" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="B107" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="B108" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="B109" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="B110" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="B111" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="B112" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="B115" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="B116" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="B117" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="B118" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="B119" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="B120" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="B121" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="B122" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="B123" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" s="9" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" t="s">
+        <v>224</v>
+      </c>
+      <c r="B125" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="B126" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="B127" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" t="s">
+        <v>223</v>
+      </c>
+      <c r="B128" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="B129" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="B130" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="B131" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="B132" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="A135" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="B136" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2">
+      <c r="B137" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2">
+      <c r="B138" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2">
+      <c r="B139" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
+      <c r="B140" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="B141" s="9" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
+      <c r="B142" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="B143" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
+      <c r="B144" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="145" spans="2:2">
+      <c r="B145" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="147" spans="2:2">
+      <c r="B147" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="148" spans="2:2">
+      <c r="B148" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="149" spans="2:2">
+      <c r="B149" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="150" spans="2:2">
+      <c r="B150" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="151" spans="2:2">
+      <c r="B151" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="152" spans="2:2">
+      <c r="B152" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="153" spans="2:2">
+      <c r="B153" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="154" spans="2:2">
+      <c r="B154" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="155" spans="2:2">
+      <c r="B155" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="157" spans="2:2">
+      <c r="B157" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="158" spans="2:2">
+      <c r="B158" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="159" spans="2:2">
+      <c r="B159" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2">
+      <c r="A161" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2">
+      <c r="B162" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2">
+      <c r="B163" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2">
+      <c r="B164" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2">
+      <c r="B165" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2">
+      <c r="B166" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2">
+      <c r="B167" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2">
+      <c r="B168" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2">
+      <c r="B169" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2">
+      <c r="B170" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2">
+      <c r="B171" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2">
+      <c r="B172" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2">
+      <c r="B173" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2">
+      <c r="B174" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2">
+      <c r="B175" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2">
+      <c r="B176" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2">
+      <c r="B177" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2">
+      <c r="B178" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2">
+      <c r="B179" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2">
+      <c r="B180" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2">
+      <c r="B181" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2">
+      <c r="B182" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2">
+      <c r="B183" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2">
+      <c r="A185" t="s">
+        <v>275</v>
+      </c>
+      <c r="B185" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2">
+      <c r="A188" s="9" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2">
+      <c r="A189" t="s">
+        <v>277</v>
+      </c>
+      <c r="B189" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2">
+      <c r="B190" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2">
+      <c r="B191" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2">
+      <c r="B192" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2">
+      <c r="B193" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2">
+      <c r="B194" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2">
+      <c r="A196" t="s">
+        <v>281</v>
+      </c>
+      <c r="B196" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2">
+      <c r="B197" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2">
+      <c r="B198" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2">
+      <c r="B200" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2">
+      <c r="B201" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2">
+      <c r="B202" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2">
+      <c r="B203" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2">
+      <c r="B204" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2">
+      <c r="B205" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2">
+      <c r="B207" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2">
+      <c r="B208" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2">
+      <c r="B209" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2">
+      <c r="B211" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2">
+      <c r="B212" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2">
+      <c r="B213" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2">
+      <c r="B214" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2">
+      <c r="A215" t="s">
+        <v>301</v>
+      </c>
+      <c r="B215" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2">
+      <c r="B216" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2">
+      <c r="A218" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2">
+      <c r="B219" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2">
+      <c r="B220" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2">
+      <c r="B221" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2">
+      <c r="B222" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2">
+      <c r="B223" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2">
+      <c r="B224" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2">
+      <c r="B225" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2">
+      <c r="B227" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2">
+      <c r="B228" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2">
+      <c r="B229" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2">
+      <c r="B230" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2">
+      <c r="A232" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2">
+      <c r="B233" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2">
+      <c r="B234" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2">
+      <c r="B235" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2">
+      <c r="B236" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2">
+      <c r="B238" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2">
+      <c r="B239" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2">
+      <c r="B240" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2">
+      <c r="A242" s="9" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2">
+      <c r="B243" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2">
+      <c r="B244" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2">
+      <c r="B245" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2">
+      <c r="B246" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2">
+      <c r="B247" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2">
+      <c r="B248" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2">
+      <c r="B249" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2">
+      <c r="B250" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2">
+      <c r="A252" s="9" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2">
+      <c r="B253" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2">
+      <c r="B254" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2">
+      <c r="B255" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2">
+      <c r="B256" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2">
+      <c r="B257" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2">
+      <c r="A259" s="9" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2">
+      <c r="B260" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2">
+      <c r="B261" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2">
+      <c r="B262" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2">
+      <c r="B263" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2">
+      <c r="B264" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2">
+      <c r="B265" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2">
+      <c r="A267" s="9" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2">
+      <c r="B268" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2">
+      <c r="B269" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2">
+      <c r="B270" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2">
+      <c r="B271" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2">
+      <c r="B272" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2">
+      <c r="B273" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2">
+      <c r="A275" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2">
+      <c r="B276" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2">
+      <c r="A277" t="s">
+        <v>358</v>
+      </c>
+      <c r="B277" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2">
+      <c r="B278" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2">
+      <c r="B279" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2">
+      <c r="B280" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2">
+      <c r="B281" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2">
+      <c r="B282" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2">
+      <c r="B283" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2">
+      <c r="B284" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2">
+      <c r="A286" s="9" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2">
+      <c r="B287" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2">
+      <c r="B288" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2">
+      <c r="B289" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2">
+      <c r="B290" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2">
+      <c r="B291" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2">
+      <c r="B292" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2">
+      <c r="B293" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2">
+      <c r="B294" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2">
+      <c r="A296" s="9" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2">
+      <c r="B297" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2">
+      <c r="B298" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2">
+      <c r="B299" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2">
+      <c r="B300" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2">
+      <c r="B301" t="s">
+        <v>356</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Some short of new pages
</commit_message>
<xml_diff>
--- a/StudyPlan.xlsx
+++ b/StudyPlan.xlsx
@@ -1,26 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rammi\Documents\Ram\Learning\ram-err404\Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306CC827-04A2-4C79-B168-CF1413EB38B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF97A621-AF09-44F4-B987-1DBEA15DB3FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{DBD4FF11-46FB-5146-978E-3349D45A0734}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{DBD4FF11-46FB-5146-978E-3349D45A0734}"/>
   </bookViews>
   <sheets>
     <sheet name="StudyPlan" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
+    <sheet name="Plan" sheetId="2" r:id="rId2"/>
+    <sheet name="Algorithms" sheetId="4" r:id="rId3"/>
     <sheet name="FAANG" sheetId="3" r:id="rId4"/>
     <sheet name="Google" sheetId="5" r:id="rId5"/>
     <sheet name="Apple" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet3" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <definedNames>
+    <definedName name="A0">FAANG!$C$1048555</definedName>
+    <definedName name="A00">FAANG!$C$1048556</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="519">
   <si>
     <t>Programming Topics</t>
   </si>
@@ -1308,13 +1313,301 @@
   </si>
   <si>
     <t>Path with minimum efforts</t>
+  </si>
+  <si>
+    <t>S.No.</t>
+  </si>
+  <si>
+    <t>feb</t>
+  </si>
+  <si>
+    <t>mar</t>
+  </si>
+  <si>
+    <t>apr</t>
+  </si>
+  <si>
+    <t>may</t>
+  </si>
+  <si>
+    <t>jun</t>
+  </si>
+  <si>
+    <t>jul</t>
+  </si>
+  <si>
+    <t>aug</t>
+  </si>
+  <si>
+    <t>sep</t>
+  </si>
+  <si>
+    <t>oct</t>
+  </si>
+  <si>
+    <t>nov</t>
+  </si>
+  <si>
+    <t>dec</t>
+  </si>
+  <si>
+    <t>jan</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Aadhar Card</t>
+  </si>
+  <si>
+    <t>Pan Card</t>
+  </si>
+  <si>
+    <t>Voter Id</t>
+  </si>
+  <si>
+    <t>Passport</t>
+  </si>
+  <si>
+    <t>10th</t>
+  </si>
+  <si>
+    <t>License (Pharmacy)</t>
+  </si>
+  <si>
+    <t>Signature</t>
+  </si>
+  <si>
+    <t>Passport Size Photo</t>
+  </si>
+  <si>
+    <t>B.Pharma (Marksheet &amp; Degree)</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>12th (Marksheet &amp; Certificate)</t>
+  </si>
+  <si>
+    <t>Cheapest Flights Within K Stops - LeetCode</t>
+  </si>
+  <si>
+    <t>Cheapest Flights within K stops</t>
+  </si>
+  <si>
+    <t>Network Delay Time - LeetCode</t>
+  </si>
+  <si>
+    <t>Network Delay Time</t>
+  </si>
+  <si>
+    <t>Number of Ways to Arrive at Destination - LeetCode</t>
+  </si>
+  <si>
+    <t>Number of Ways to Arrive at Destination</t>
+  </si>
+  <si>
+    <t>Minimum Multiplications to reach End | Practice | GeeksforGeeks</t>
+  </si>
+  <si>
+    <t>Minimum multiplication to reach end</t>
+  </si>
+  <si>
+    <t>MST &amp; DSU</t>
+  </si>
+  <si>
+    <t>Minimum Spanning Tree | Practice | GeeksforGeeks</t>
+  </si>
+  <si>
+    <t>Disjoint Set</t>
+  </si>
+  <si>
+    <t>Disjoint Set | Union by Rank | Union by Size | Path Compression: G-46 - Tutorial (takeuforward.org)</t>
+  </si>
+  <si>
+    <t>Krushkal's Algorithm</t>
+  </si>
+  <si>
+    <t>Number of Operations to Make Network Connected - LeetCode</t>
+  </si>
+  <si>
+    <t>Number of operations to make network connected</t>
+  </si>
+  <si>
+    <t>Most Stones Removed with Same Row or Column - LeetCode</t>
+  </si>
+  <si>
+    <t>Accounts Merge - LeetCode</t>
+  </si>
+  <si>
+    <t>Number of Islands - II - Online Queries - DSU: G-51 - Tutorial (takeuforward.org)</t>
+  </si>
+  <si>
+    <t>Making A Large Island - LeetCode</t>
+  </si>
+  <si>
+    <t>Swim in Rising Water - LeetCode</t>
+  </si>
+  <si>
+    <t>Bridges/Tarjan</t>
+  </si>
+  <si>
+    <t>Critical Connections in a Network - LeetCode</t>
+  </si>
+  <si>
+    <t>Bridges in Graph / Critical Connections in a Network</t>
+  </si>
+  <si>
+    <t>Articulation Point - I | Practice | GeeksforGeeks</t>
+  </si>
+  <si>
+    <t>Articulation Point</t>
+  </si>
+  <si>
+    <t>Kosaraju's Algo</t>
+  </si>
+  <si>
+    <t>Strongly Connected Components (Kosaraju's Algo) | Practice | GeeksforGeeks</t>
+  </si>
+  <si>
+    <t>Kosaraju's Algorithm / Strongly Connected Components</t>
+  </si>
+  <si>
+    <t>DFS / BFS</t>
+  </si>
+  <si>
+    <t>Tree's / BST</t>
+  </si>
+  <si>
+    <t>Most Stones Removed with Same Row or Column</t>
+  </si>
+  <si>
+    <t>Accounts Merge</t>
+  </si>
+  <si>
+    <t>Making a Large Island</t>
+  </si>
+  <si>
+    <t>S.No</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>Minimum Area Rectangle</t>
+  </si>
+  <si>
+    <t>Minimum Area Rectangle 2</t>
+  </si>
+  <si>
+    <t>Minimum Area Rectangle - LeetCode</t>
+  </si>
+  <si>
+    <t>Minimum Area Rectangle II - LeetCode</t>
+  </si>
+  <si>
+    <t>Shortest Path in a Grid with Obstacles Elimination - LeetCode</t>
+  </si>
+  <si>
+    <t>Find All Duplicates in an Array - LeetCode</t>
+  </si>
+  <si>
+    <t>Basic Calculator - LeetCode</t>
+  </si>
+  <si>
+    <t>Basic Calculator IV - LeetCode</t>
+  </si>
+  <si>
+    <t>Text Justification - LeetCode</t>
+  </si>
+  <si>
+    <t>Lowest Common Ancestor of a Binary Tree - LeetCode</t>
+  </si>
+  <si>
+    <t>Largest Plus Sign - LeetCode</t>
+  </si>
+  <si>
+    <t>Minimum Time Difference - LeetCode</t>
+  </si>
+  <si>
+    <t>Longest Increasing Path in a Matrix - LeetCode</t>
+  </si>
+  <si>
+    <t>String to Integer (atoi) - LeetCode</t>
+  </si>
+  <si>
+    <t>Step-By-Step Directions From a Binary Tree Node to Another - LeetCode</t>
+  </si>
+  <si>
+    <t>Remove All Adjacent Duplicates In String - LeetCode</t>
+  </si>
+  <si>
+    <t>Simplify Path - LeetCode</t>
+  </si>
+  <si>
+    <t>Letter Combinations of a Phone Number - LeetCode</t>
+  </si>
+  <si>
+    <t>Kth Largest Element in an Array - LeetCode</t>
+  </si>
+  <si>
+    <t>Number of Islands - LeetCode</t>
+  </si>
+  <si>
+    <t>Max Area of Island - LeetCode</t>
+  </si>
+  <si>
+    <t>Find leaves of binary tree</t>
+  </si>
+  <si>
+    <t>Minimum Number of Refueling Stops - LeetCode</t>
+  </si>
+  <si>
+    <t>Kill process</t>
+  </si>
+  <si>
+    <t>Find Median from Data Stream - LeetCode</t>
+  </si>
+  <si>
+    <t>Split Array Largest Sum - LeetCode</t>
+  </si>
+  <si>
+    <t>Car Pooling - LeetCode</t>
+  </si>
+  <si>
+    <t>Find All People With Secret - LeetCode</t>
+  </si>
+  <si>
+    <t>Evaluate Reverse Polish Notation - LeetCode</t>
+  </si>
+  <si>
+    <t>Logger Rate Limiter</t>
+  </si>
+  <si>
+    <t>Validate Binary Tree Nodes - LeetCode</t>
+  </si>
+  <si>
+    <t>Clone Graph - LeetCode</t>
+  </si>
+  <si>
+    <t>Robot Room Cleaner</t>
+  </si>
+  <si>
+    <t>Valid Word Abbriviation</t>
+  </si>
+  <si>
+    <t>Number of Visible People in a Queue - LeetCode</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1380,6 +1673,20 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1519,7 +1826,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1554,10 +1861,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2365,10 +2676,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="16.5" thickBot="1">
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="22"/>
+      <c r="C2" s="23"/>
     </row>
     <row r="3" spans="2:5" ht="17.25" thickTop="1" thickBot="1">
       <c r="B3" s="1" t="s">
@@ -2550,7 +2861,7 @@
   <dimension ref="A1:C301"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B121" sqref="B121"/>
+      <selection activeCell="B301" sqref="B301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -3954,38 +4265,39 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{777FF9AE-CAA8-7C48-8B5E-839EF7342066}">
-  <dimension ref="A1:H108"/>
+  <dimension ref="A1:I108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21"/>
   <cols>
     <col min="1" max="1" width="17.625" style="18" customWidth="1"/>
-    <col min="2" max="2" width="11.625" style="18" customWidth="1"/>
-    <col min="3" max="3" width="52.625" style="18" customWidth="1"/>
-    <col min="4" max="4" width="81.5" style="18" customWidth="1"/>
-    <col min="5" max="5" width="18.75" style="18" customWidth="1"/>
-    <col min="6" max="6" width="19.375" style="18" customWidth="1"/>
-    <col min="7" max="7" width="20.75" style="18" customWidth="1"/>
-    <col min="8" max="8" width="21.625" style="18" customWidth="1"/>
-    <col min="9" max="16384" width="10.875" style="18"/>
+    <col min="2" max="3" width="11.625" style="18" customWidth="1"/>
+    <col min="4" max="4" width="52.625" style="18" customWidth="1"/>
+    <col min="5" max="5" width="81.5" style="18" customWidth="1"/>
+    <col min="6" max="6" width="18.75" style="18" customWidth="1"/>
+    <col min="7" max="7" width="19.375" style="18" customWidth="1"/>
+    <col min="8" max="8" width="20.75" style="18" customWidth="1"/>
+    <col min="9" max="9" width="21.625" style="18" customWidth="1"/>
+    <col min="10" max="16384" width="10.875" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26.25">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:9" ht="26.25">
+      <c r="A1" s="24" t="s">
         <v>411</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="19" t="s">
         <v>83</v>
       </c>
@@ -3993,1018 +4305,1704 @@
         <v>96</v>
       </c>
       <c r="C3" s="19" t="s">
+        <v>423</v>
+      </c>
+      <c r="D3" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="E3" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="F3" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="G3" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="H3" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="H3" s="19"/>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3" s="19"/>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="20" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="21">
         <v>45421</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="21" t="s">
         <v>377</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="E4" s="17" t="s">
         <v>376</v>
       </c>
-      <c r="E4"/>
       <c r="F4"/>
       <c r="G4"/>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="H4"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="18" t="s">
+        <v>476</v>
+      </c>
       <c r="B5"/>
-      <c r="C5" t="s">
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
         <v>378</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="E5" s="17" t="s">
         <v>379</v>
       </c>
-      <c r="E5"/>
       <c r="F5"/>
       <c r="G5"/>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="H5"/>
+    </row>
+    <row r="6" spans="1:9">
       <c r="B6"/>
-      <c r="C6" t="s">
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
         <v>103</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="E6" s="17" t="s">
         <v>380</v>
       </c>
-      <c r="E6"/>
       <c r="F6"/>
       <c r="G6"/>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="H6"/>
+    </row>
+    <row r="7" spans="1:9">
       <c r="B7"/>
-      <c r="C7" t="s">
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
         <v>381</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="E7" s="17" t="s">
         <v>382</v>
       </c>
-      <c r="E7"/>
       <c r="F7"/>
       <c r="G7"/>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="H7"/>
+    </row>
+    <row r="8" spans="1:9">
       <c r="B8"/>
-      <c r="C8" t="s">
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
         <v>383</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="E8" s="17" t="s">
         <v>384</v>
       </c>
-      <c r="E8"/>
       <c r="F8"/>
       <c r="G8"/>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="H8"/>
+    </row>
+    <row r="9" spans="1:9">
       <c r="B9"/>
-      <c r="C9" t="s">
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
         <v>386</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="E9" s="17" t="s">
         <v>385</v>
       </c>
-      <c r="E9"/>
       <c r="F9"/>
       <c r="G9"/>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="H9"/>
+    </row>
+    <row r="10" spans="1:9">
       <c r="B10"/>
-      <c r="C10" t="s">
+      <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
         <v>388</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="E10" s="17" t="s">
         <v>387</v>
       </c>
-      <c r="E10"/>
       <c r="F10"/>
       <c r="G10"/>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="H10"/>
+    </row>
+    <row r="11" spans="1:9">
       <c r="B11"/>
-      <c r="C11" t="s">
+      <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
         <v>389</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="E11" s="17" t="s">
         <v>390</v>
       </c>
-      <c r="E11"/>
       <c r="F11"/>
       <c r="G11"/>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="H11"/>
+    </row>
+    <row r="12" spans="1:9">
       <c r="B12"/>
-      <c r="C12" t="s">
+      <c r="C12">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
         <v>392</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="E12" s="17" t="s">
         <v>391</v>
       </c>
-      <c r="E12"/>
       <c r="F12"/>
       <c r="G12"/>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="H12"/>
+    </row>
+    <row r="13" spans="1:9">
       <c r="B13"/>
-      <c r="C13" t="s">
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
         <v>394</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="E13" s="17" t="s">
         <v>393</v>
       </c>
-      <c r="E13"/>
       <c r="F13"/>
       <c r="G13"/>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="H13"/>
+    </row>
+    <row r="14" spans="1:9">
       <c r="B14"/>
-      <c r="C14" t="s">
+      <c r="C14">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
         <v>396</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="E14" s="17" t="s">
         <v>395</v>
       </c>
-      <c r="E14"/>
       <c r="F14"/>
       <c r="G14"/>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="H14"/>
+    </row>
+    <row r="15" spans="1:9">
       <c r="B15" s="21">
         <v>45425</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
         <v>398</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="E15" s="17" t="s">
         <v>397</v>
       </c>
-      <c r="E15"/>
       <c r="F15"/>
       <c r="G15"/>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="H15"/>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" s="18" t="s">
         <v>399</v>
       </c>
       <c r="B16"/>
-      <c r="C16" t="s">
+      <c r="C16">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s">
         <v>389</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="E16" s="17" t="s">
         <v>400</v>
       </c>
-      <c r="E16"/>
       <c r="F16"/>
       <c r="G16"/>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="H16"/>
+    </row>
+    <row r="17" spans="1:8">
       <c r="B17"/>
-      <c r="C17" t="s">
+      <c r="C17">
+        <v>14</v>
+      </c>
+      <c r="D17" t="s">
         <v>401</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="E17" s="17" t="s">
         <v>400</v>
       </c>
-      <c r="E17"/>
       <c r="F17"/>
       <c r="G17"/>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="H17"/>
+    </row>
+    <row r="18" spans="1:8">
       <c r="B18" s="21">
         <v>45426</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18">
+        <v>15</v>
+      </c>
+      <c r="D18" t="s">
         <v>403</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="E18" s="17" t="s">
         <v>402</v>
       </c>
-      <c r="E18"/>
       <c r="F18"/>
       <c r="G18"/>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="H18"/>
+    </row>
+    <row r="19" spans="1:8">
       <c r="B19" s="21">
         <v>45427</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19">
+        <v>16</v>
+      </c>
+      <c r="D19" t="s">
         <v>405</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="E19" s="17" t="s">
         <v>404</v>
       </c>
-      <c r="E19"/>
       <c r="F19"/>
       <c r="G19"/>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="H19"/>
+    </row>
+    <row r="20" spans="1:8">
       <c r="B20"/>
-      <c r="C20" t="s">
+      <c r="C20">
+        <v>17</v>
+      </c>
+      <c r="D20" t="s">
         <v>407</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="E20" s="17" t="s">
         <v>406</v>
       </c>
-      <c r="E20"/>
       <c r="F20"/>
       <c r="G20"/>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="H20"/>
+    </row>
+    <row r="21" spans="1:8">
       <c r="B21"/>
       <c r="C21"/>
-      <c r="D21" s="17"/>
-      <c r="E21"/>
+      <c r="D21"/>
+      <c r="E21" s="17"/>
       <c r="F21"/>
       <c r="G21"/>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="H21"/>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="18" t="s">
         <v>412</v>
       </c>
       <c r="B22"/>
-      <c r="C22" t="s">
+      <c r="C22">
+        <v>18</v>
+      </c>
+      <c r="D22" t="s">
         <v>414</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="E22" s="17" t="s">
         <v>413</v>
       </c>
-      <c r="E22"/>
       <c r="F22"/>
       <c r="G22"/>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="H22"/>
+    </row>
+    <row r="23" spans="1:8">
       <c r="B23"/>
       <c r="C23"/>
-      <c r="D23" s="17"/>
-      <c r="E23"/>
+      <c r="D23"/>
+      <c r="E23" s="17"/>
       <c r="F23"/>
       <c r="G23"/>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="H23"/>
+    </row>
+    <row r="24" spans="1:8">
       <c r="B24"/>
       <c r="C24"/>
-      <c r="D24" s="17"/>
-      <c r="E24"/>
+      <c r="D24"/>
+      <c r="E24" s="17"/>
       <c r="F24"/>
       <c r="G24"/>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="H24"/>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="18" t="s">
         <v>408</v>
       </c>
       <c r="B25" s="21">
         <v>45428</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25">
+        <v>19</v>
+      </c>
+      <c r="D25" t="s">
         <v>410</v>
       </c>
-      <c r="D25" s="17" t="s">
+      <c r="E25" s="17" t="s">
         <v>409</v>
       </c>
-      <c r="E25"/>
       <c r="F25"/>
       <c r="G25"/>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="H25"/>
+    </row>
+    <row r="26" spans="1:8">
       <c r="B26"/>
-      <c r="C26" t="s">
+      <c r="C26">
+        <v>20</v>
+      </c>
+      <c r="D26" t="s">
         <v>416</v>
       </c>
-      <c r="D26" s="17" t="s">
+      <c r="E26" s="17" t="s">
         <v>415</v>
       </c>
-      <c r="E26"/>
       <c r="F26"/>
       <c r="G26"/>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="H26"/>
+    </row>
+    <row r="27" spans="1:8">
       <c r="B27"/>
-      <c r="C27" t="s">
+      <c r="C27">
+        <v>21</v>
+      </c>
+      <c r="D27" t="s">
         <v>418</v>
       </c>
-      <c r="D27" s="17" t="s">
+      <c r="E27" s="17" t="s">
         <v>417</v>
       </c>
-      <c r="E27"/>
       <c r="F27"/>
       <c r="G27"/>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="H27"/>
+    </row>
+    <row r="28" spans="1:8">
       <c r="B28"/>
-      <c r="C28" t="s">
+      <c r="C28">
+        <v>22</v>
+      </c>
+      <c r="D28" t="s">
         <v>420</v>
       </c>
-      <c r="D28" s="17" t="s">
+      <c r="E28" s="17" t="s">
         <v>419</v>
       </c>
-      <c r="E28"/>
       <c r="F28"/>
       <c r="G28"/>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="B29"/>
-      <c r="C29" t="s">
+      <c r="H28"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="B29" s="21">
+        <v>45433</v>
+      </c>
+      <c r="C29">
+        <v>23</v>
+      </c>
+      <c r="D29" t="s">
         <v>422</v>
       </c>
-      <c r="D29" s="17" t="s">
+      <c r="E29" s="17" t="s">
         <v>421</v>
       </c>
-      <c r="E29"/>
       <c r="F29"/>
       <c r="G29"/>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="B30"/>
-      <c r="C30"/>
-      <c r="D30"/>
-      <c r="E30"/>
+      <c r="H29"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="B30" s="21">
+        <v>45435</v>
+      </c>
+      <c r="C30">
+        <v>24</v>
+      </c>
+      <c r="D30" t="s">
+        <v>449</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>448</v>
+      </c>
       <c r="F30"/>
       <c r="G30"/>
-    </row>
-    <row r="31" spans="1:7">
+      <c r="H30"/>
+    </row>
+    <row r="31" spans="1:8">
       <c r="B31"/>
-      <c r="C31"/>
-      <c r="D31"/>
-      <c r="E31"/>
+      <c r="C31">
+        <v>25</v>
+      </c>
+      <c r="D31" t="s">
+        <v>451</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>450</v>
+      </c>
       <c r="F31"/>
       <c r="G31"/>
-    </row>
-    <row r="32" spans="1:7">
+      <c r="H31"/>
+    </row>
+    <row r="32" spans="1:8">
       <c r="B32"/>
-      <c r="C32"/>
-      <c r="D32"/>
-      <c r="E32"/>
+      <c r="C32">
+        <v>26</v>
+      </c>
+      <c r="D32" t="s">
+        <v>453</v>
+      </c>
+      <c r="E32" s="17" t="s">
+        <v>452</v>
+      </c>
       <c r="F32"/>
       <c r="G32"/>
-    </row>
-    <row r="33" spans="2:7">
+      <c r="H32"/>
+    </row>
+    <row r="33" spans="1:8">
       <c r="B33"/>
-      <c r="C33"/>
-      <c r="D33"/>
-      <c r="E33"/>
+      <c r="C33">
+        <v>27</v>
+      </c>
+      <c r="D33" t="s">
+        <v>455</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>454</v>
+      </c>
       <c r="F33"/>
       <c r="G33"/>
-    </row>
-    <row r="34" spans="2:7">
+      <c r="H33"/>
+    </row>
+    <row r="34" spans="1:8">
       <c r="B34"/>
-      <c r="C34"/>
+      <c r="C34">
+        <v>28</v>
+      </c>
       <c r="D34"/>
       <c r="E34"/>
       <c r="F34"/>
       <c r="G34"/>
-    </row>
-    <row r="35" spans="2:7">
+      <c r="H34"/>
+    </row>
+    <row r="35" spans="1:8">
       <c r="B35"/>
-      <c r="C35"/>
+      <c r="C35">
+        <v>29</v>
+      </c>
       <c r="D35"/>
       <c r="E35"/>
       <c r="F35"/>
       <c r="G35"/>
-    </row>
-    <row r="36" spans="2:7">
+      <c r="H35"/>
+    </row>
+    <row r="36" spans="1:8">
       <c r="B36"/>
-      <c r="C36"/>
+      <c r="C36">
+        <v>30</v>
+      </c>
       <c r="D36"/>
       <c r="E36"/>
       <c r="F36"/>
       <c r="G36"/>
-    </row>
-    <row r="37" spans="2:7">
+      <c r="H36"/>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="18" t="s">
+        <v>456</v>
+      </c>
       <c r="B37"/>
       <c r="C37"/>
       <c r="D37"/>
       <c r="E37"/>
       <c r="F37"/>
       <c r="G37"/>
-    </row>
-    <row r="38" spans="2:7">
-      <c r="B38"/>
-      <c r="C38"/>
-      <c r="D38"/>
-      <c r="E38"/>
+      <c r="H37"/>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="B38" s="21">
+        <v>45443</v>
+      </c>
+      <c r="C38">
+        <v>31</v>
+      </c>
+      <c r="D38" t="s">
+        <v>118</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>457</v>
+      </c>
       <c r="F38"/>
       <c r="G38"/>
-    </row>
-    <row r="39" spans="2:7">
+      <c r="H38"/>
+    </row>
+    <row r="39" spans="1:8">
       <c r="B39"/>
-      <c r="C39"/>
-      <c r="D39"/>
-      <c r="E39"/>
+      <c r="C39">
+        <v>32</v>
+      </c>
+      <c r="D39" t="s">
+        <v>119</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>457</v>
+      </c>
       <c r="F39"/>
       <c r="G39"/>
-    </row>
-    <row r="40" spans="2:7">
+      <c r="H39"/>
+    </row>
+    <row r="40" spans="1:8">
       <c r="B40"/>
-      <c r="C40"/>
-      <c r="D40"/>
-      <c r="E40"/>
+      <c r="C40">
+        <v>33</v>
+      </c>
+      <c r="D40" t="s">
+        <v>458</v>
+      </c>
+      <c r="E40" s="17" t="s">
+        <v>459</v>
+      </c>
       <c r="F40"/>
       <c r="G40"/>
-    </row>
-    <row r="41" spans="2:7">
+      <c r="H40"/>
+    </row>
+    <row r="41" spans="1:8">
       <c r="B41"/>
-      <c r="C41"/>
-      <c r="D41"/>
-      <c r="E41"/>
+      <c r="C41">
+        <v>34</v>
+      </c>
+      <c r="D41" t="s">
+        <v>460</v>
+      </c>
+      <c r="E41" s="17" t="s">
+        <v>457</v>
+      </c>
       <c r="F41"/>
       <c r="G41"/>
-    </row>
-    <row r="42" spans="2:7">
+      <c r="H41"/>
+    </row>
+    <row r="42" spans="1:8">
       <c r="B42"/>
-      <c r="C42"/>
-      <c r="D42"/>
-      <c r="E42"/>
+      <c r="C42">
+        <v>35</v>
+      </c>
+      <c r="D42" t="s">
+        <v>462</v>
+      </c>
+      <c r="E42" s="17" t="s">
+        <v>461</v>
+      </c>
       <c r="F42"/>
       <c r="G42"/>
-    </row>
-    <row r="43" spans="2:7">
-      <c r="B43"/>
-      <c r="C43"/>
-      <c r="D43"/>
-      <c r="E43"/>
+      <c r="H42"/>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="B43" s="21">
+        <v>45444</v>
+      </c>
+      <c r="C43">
+        <v>36</v>
+      </c>
+      <c r="D43" t="s">
+        <v>478</v>
+      </c>
+      <c r="E43" s="17" t="s">
+        <v>463</v>
+      </c>
       <c r="F43"/>
       <c r="G43"/>
-    </row>
-    <row r="44" spans="2:7">
-      <c r="B44"/>
-      <c r="C44"/>
-      <c r="D44"/>
-      <c r="E44"/>
+      <c r="H43"/>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="B44" s="21">
+        <v>45445</v>
+      </c>
+      <c r="C44">
+        <v>37</v>
+      </c>
+      <c r="D44" t="s">
+        <v>479</v>
+      </c>
+      <c r="E44" s="17" t="s">
+        <v>464</v>
+      </c>
       <c r="F44"/>
       <c r="G44"/>
-    </row>
-    <row r="45" spans="2:7">
+      <c r="H44"/>
+    </row>
+    <row r="45" spans="1:8">
       <c r="B45"/>
-      <c r="C45"/>
+      <c r="C45">
+        <v>38</v>
+      </c>
       <c r="D45"/>
-      <c r="E45"/>
+      <c r="E45" s="17" t="s">
+        <v>465</v>
+      </c>
       <c r="F45"/>
       <c r="G45"/>
-    </row>
-    <row r="46" spans="2:7">
+      <c r="H45"/>
+    </row>
+    <row r="46" spans="1:8">
       <c r="B46"/>
-      <c r="C46"/>
-      <c r="D46"/>
-      <c r="E46"/>
+      <c r="C46">
+        <v>39</v>
+      </c>
+      <c r="D46" t="s">
+        <v>480</v>
+      </c>
+      <c r="E46" s="17" t="s">
+        <v>466</v>
+      </c>
       <c r="F46"/>
       <c r="G46"/>
-    </row>
-    <row r="47" spans="2:7">
+      <c r="H46"/>
+    </row>
+    <row r="47" spans="1:8">
       <c r="B47"/>
-      <c r="C47"/>
+      <c r="C47">
+        <v>40</v>
+      </c>
       <c r="D47"/>
-      <c r="E47"/>
+      <c r="E47" s="17" t="s">
+        <v>467</v>
+      </c>
       <c r="F47"/>
       <c r="G47"/>
-    </row>
-    <row r="48" spans="2:7">
+      <c r="H47"/>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="18" t="s">
+        <v>468</v>
+      </c>
       <c r="B48"/>
       <c r="C48"/>
       <c r="D48"/>
       <c r="E48"/>
       <c r="F48"/>
       <c r="G48"/>
-    </row>
-    <row r="49" spans="2:7">
+      <c r="H48"/>
+    </row>
+    <row r="49" spans="1:8">
       <c r="B49"/>
-      <c r="C49"/>
-      <c r="D49"/>
-      <c r="E49"/>
+      <c r="C49">
+        <v>41</v>
+      </c>
+      <c r="D49" t="s">
+        <v>470</v>
+      </c>
+      <c r="E49" s="17" t="s">
+        <v>469</v>
+      </c>
       <c r="F49"/>
       <c r="G49"/>
-    </row>
-    <row r="50" spans="2:7">
+      <c r="H49"/>
+    </row>
+    <row r="50" spans="1:8">
       <c r="B50"/>
-      <c r="C50"/>
-      <c r="D50"/>
-      <c r="E50"/>
+      <c r="C50">
+        <v>42</v>
+      </c>
+      <c r="D50" t="s">
+        <v>472</v>
+      </c>
+      <c r="E50" s="17" t="s">
+        <v>471</v>
+      </c>
       <c r="F50"/>
       <c r="G50"/>
-    </row>
-    <row r="51" spans="2:7">
+      <c r="H50"/>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="18" t="s">
+        <v>473</v>
+      </c>
       <c r="B51"/>
       <c r="C51"/>
       <c r="D51"/>
       <c r="E51"/>
       <c r="F51"/>
       <c r="G51"/>
-    </row>
-    <row r="52" spans="2:7">
-      <c r="B52"/>
-      <c r="C52"/>
-      <c r="D52"/>
-      <c r="E52"/>
+      <c r="H51"/>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="B52" s="21">
+        <v>45445</v>
+      </c>
+      <c r="C52">
+        <v>43</v>
+      </c>
+      <c r="D52" t="s">
+        <v>475</v>
+      </c>
+      <c r="E52" s="17" t="s">
+        <v>474</v>
+      </c>
       <c r="F52"/>
       <c r="G52"/>
-    </row>
-    <row r="53" spans="2:7">
+      <c r="H52"/>
+    </row>
+    <row r="53" spans="1:8">
       <c r="B53"/>
       <c r="C53"/>
       <c r="D53"/>
       <c r="E53"/>
       <c r="F53"/>
       <c r="G53"/>
-    </row>
-    <row r="54" spans="2:7">
+      <c r="H53"/>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="18" t="s">
+        <v>477</v>
+      </c>
       <c r="B54"/>
       <c r="C54"/>
       <c r="D54"/>
       <c r="E54"/>
       <c r="F54"/>
       <c r="G54"/>
-    </row>
-    <row r="55" spans="2:7">
+      <c r="H54"/>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" s="18" t="s">
+        <v>277</v>
+      </c>
       <c r="B55"/>
-      <c r="C55"/>
-      <c r="D55"/>
+      <c r="C55">
+        <v>44</v>
+      </c>
+      <c r="D55" t="s">
+        <v>279</v>
+      </c>
       <c r="E55"/>
       <c r="F55"/>
       <c r="G55"/>
-    </row>
-    <row r="56" spans="2:7">
+      <c r="H55"/>
+    </row>
+    <row r="56" spans="1:8">
       <c r="B56"/>
-      <c r="C56"/>
-      <c r="D56"/>
+      <c r="C56">
+        <v>45</v>
+      </c>
+      <c r="D56" t="s">
+        <v>278</v>
+      </c>
       <c r="E56"/>
       <c r="F56"/>
       <c r="G56"/>
-    </row>
-    <row r="57" spans="2:7">
+      <c r="H56"/>
+    </row>
+    <row r="57" spans="1:8">
       <c r="B57"/>
-      <c r="C57"/>
-      <c r="D57"/>
+      <c r="C57">
+        <v>46</v>
+      </c>
+      <c r="D57" t="s">
+        <v>287</v>
+      </c>
       <c r="E57"/>
       <c r="F57"/>
       <c r="G57"/>
-    </row>
-    <row r="58" spans="2:7">
+      <c r="H57"/>
+    </row>
+    <row r="58" spans="1:8">
       <c r="B58"/>
-      <c r="C58"/>
-      <c r="D58"/>
+      <c r="C58">
+        <v>47</v>
+      </c>
+      <c r="D58" t="s">
+        <v>288</v>
+      </c>
       <c r="E58"/>
       <c r="F58"/>
       <c r="G58"/>
-    </row>
-    <row r="59" spans="2:7">
+      <c r="H58"/>
+    </row>
+    <row r="59" spans="1:8">
       <c r="B59"/>
-      <c r="C59"/>
-      <c r="D59"/>
+      <c r="C59">
+        <v>48</v>
+      </c>
+      <c r="D59" t="s">
+        <v>289</v>
+      </c>
       <c r="E59"/>
       <c r="F59"/>
       <c r="G59"/>
-    </row>
-    <row r="60" spans="2:7">
+      <c r="H59"/>
+    </row>
+    <row r="60" spans="1:8">
       <c r="B60"/>
-      <c r="C60"/>
-      <c r="D60"/>
+      <c r="C60">
+        <v>49</v>
+      </c>
+      <c r="D60" t="s">
+        <v>302</v>
+      </c>
       <c r="E60"/>
       <c r="F60"/>
       <c r="G60"/>
-    </row>
-    <row r="61" spans="2:7">
+      <c r="H60"/>
+    </row>
+    <row r="61" spans="1:8">
       <c r="B61"/>
       <c r="C61"/>
       <c r="D61"/>
       <c r="E61"/>
       <c r="F61"/>
       <c r="G61"/>
-    </row>
-    <row r="62" spans="2:7">
+      <c r="H61"/>
+    </row>
+    <row r="62" spans="1:8">
       <c r="B62"/>
       <c r="C62"/>
       <c r="D62"/>
       <c r="E62"/>
       <c r="F62"/>
       <c r="G62"/>
-    </row>
-    <row r="63" spans="2:7">
+      <c r="H62"/>
+    </row>
+    <row r="63" spans="1:8">
       <c r="B63"/>
       <c r="C63"/>
       <c r="D63"/>
       <c r="E63"/>
       <c r="F63"/>
       <c r="G63"/>
-    </row>
-    <row r="64" spans="2:7">
+      <c r="H63"/>
+    </row>
+    <row r="64" spans="1:8">
       <c r="B64"/>
       <c r="C64"/>
       <c r="D64"/>
       <c r="E64"/>
       <c r="F64"/>
       <c r="G64"/>
-    </row>
-    <row r="65" spans="2:7">
+      <c r="H64"/>
+    </row>
+    <row r="65" spans="2:8">
       <c r="B65"/>
       <c r="C65"/>
       <c r="D65"/>
       <c r="E65"/>
       <c r="F65"/>
       <c r="G65"/>
-    </row>
-    <row r="66" spans="2:7">
+      <c r="H65"/>
+    </row>
+    <row r="66" spans="2:8">
       <c r="B66"/>
       <c r="C66"/>
       <c r="D66"/>
       <c r="E66"/>
       <c r="F66"/>
       <c r="G66"/>
-    </row>
-    <row r="67" spans="2:7">
+      <c r="H66"/>
+    </row>
+    <row r="67" spans="2:8">
       <c r="B67"/>
       <c r="C67"/>
       <c r="D67"/>
       <c r="E67"/>
       <c r="F67"/>
       <c r="G67"/>
-    </row>
-    <row r="68" spans="2:7">
+      <c r="H67"/>
+    </row>
+    <row r="68" spans="2:8">
       <c r="B68"/>
       <c r="C68"/>
       <c r="D68"/>
       <c r="E68"/>
       <c r="F68"/>
       <c r="G68"/>
-    </row>
-    <row r="69" spans="2:7">
+      <c r="H68"/>
+    </row>
+    <row r="69" spans="2:8">
       <c r="B69"/>
       <c r="C69"/>
       <c r="D69"/>
       <c r="E69"/>
       <c r="F69"/>
       <c r="G69"/>
-    </row>
-    <row r="70" spans="2:7">
+      <c r="H69"/>
+    </row>
+    <row r="70" spans="2:8">
       <c r="B70"/>
       <c r="C70"/>
       <c r="D70"/>
       <c r="E70"/>
       <c r="F70"/>
       <c r="G70"/>
-    </row>
-    <row r="71" spans="2:7">
+      <c r="H70"/>
+    </row>
+    <row r="71" spans="2:8">
       <c r="B71"/>
       <c r="C71"/>
       <c r="D71"/>
       <c r="E71"/>
       <c r="F71"/>
       <c r="G71"/>
-    </row>
-    <row r="72" spans="2:7">
+      <c r="H71"/>
+    </row>
+    <row r="72" spans="2:8">
       <c r="B72"/>
       <c r="C72"/>
       <c r="D72"/>
       <c r="E72"/>
       <c r="F72"/>
       <c r="G72"/>
-    </row>
-    <row r="73" spans="2:7">
+      <c r="H72"/>
+    </row>
+    <row r="73" spans="2:8">
       <c r="B73"/>
       <c r="C73"/>
       <c r="D73"/>
       <c r="E73"/>
       <c r="F73"/>
       <c r="G73"/>
-    </row>
-    <row r="74" spans="2:7">
+      <c r="H73"/>
+    </row>
+    <row r="74" spans="2:8">
       <c r="B74"/>
       <c r="C74"/>
       <c r="D74"/>
       <c r="E74"/>
       <c r="F74"/>
       <c r="G74"/>
-    </row>
-    <row r="75" spans="2:7">
+      <c r="H74"/>
+    </row>
+    <row r="75" spans="2:8">
       <c r="B75"/>
       <c r="C75"/>
       <c r="D75"/>
       <c r="E75"/>
       <c r="F75"/>
       <c r="G75"/>
-    </row>
-    <row r="76" spans="2:7">
+      <c r="H75"/>
+    </row>
+    <row r="76" spans="2:8">
       <c r="B76"/>
       <c r="C76"/>
       <c r="D76"/>
       <c r="E76"/>
       <c r="F76"/>
       <c r="G76"/>
-    </row>
-    <row r="77" spans="2:7">
+      <c r="H76"/>
+    </row>
+    <row r="77" spans="2:8">
       <c r="B77"/>
       <c r="C77"/>
       <c r="D77"/>
       <c r="E77"/>
       <c r="F77"/>
       <c r="G77"/>
-    </row>
-    <row r="78" spans="2:7">
+      <c r="H77"/>
+    </row>
+    <row r="78" spans="2:8">
       <c r="B78"/>
       <c r="C78"/>
       <c r="D78"/>
       <c r="E78"/>
       <c r="F78"/>
       <c r="G78"/>
-    </row>
-    <row r="79" spans="2:7">
+      <c r="H78"/>
+    </row>
+    <row r="79" spans="2:8">
       <c r="B79"/>
       <c r="C79"/>
       <c r="D79"/>
       <c r="E79"/>
       <c r="F79"/>
       <c r="G79"/>
-    </row>
-    <row r="80" spans="2:7">
+      <c r="H79"/>
+    </row>
+    <row r="80" spans="2:8">
       <c r="B80"/>
       <c r="C80"/>
       <c r="D80"/>
       <c r="E80"/>
       <c r="F80"/>
       <c r="G80"/>
-    </row>
-    <row r="81" spans="2:7">
+      <c r="H80"/>
+    </row>
+    <row r="81" spans="2:8">
       <c r="B81"/>
       <c r="C81"/>
       <c r="D81"/>
       <c r="E81"/>
       <c r="F81"/>
       <c r="G81"/>
-    </row>
-    <row r="82" spans="2:7">
+      <c r="H81"/>
+    </row>
+    <row r="82" spans="2:8">
       <c r="B82"/>
       <c r="C82"/>
       <c r="D82"/>
       <c r="E82"/>
       <c r="F82"/>
       <c r="G82"/>
-    </row>
-    <row r="83" spans="2:7">
+      <c r="H82"/>
+    </row>
+    <row r="83" spans="2:8">
       <c r="B83"/>
       <c r="C83"/>
       <c r="D83"/>
       <c r="E83"/>
       <c r="F83"/>
       <c r="G83"/>
-    </row>
-    <row r="84" spans="2:7">
+      <c r="H83"/>
+    </row>
+    <row r="84" spans="2:8">
       <c r="B84"/>
       <c r="C84"/>
       <c r="D84"/>
       <c r="E84"/>
       <c r="F84"/>
       <c r="G84"/>
-    </row>
-    <row r="85" spans="2:7">
+      <c r="H84"/>
+    </row>
+    <row r="85" spans="2:8">
       <c r="B85"/>
       <c r="C85"/>
       <c r="D85"/>
       <c r="E85"/>
       <c r="F85"/>
       <c r="G85"/>
-    </row>
-    <row r="86" spans="2:7">
+      <c r="H85"/>
+    </row>
+    <row r="86" spans="2:8">
       <c r="B86"/>
       <c r="C86"/>
       <c r="D86"/>
       <c r="E86"/>
       <c r="F86"/>
       <c r="G86"/>
-    </row>
-    <row r="87" spans="2:7">
+      <c r="H86"/>
+    </row>
+    <row r="87" spans="2:8">
       <c r="B87"/>
       <c r="C87"/>
       <c r="D87"/>
       <c r="E87"/>
       <c r="F87"/>
       <c r="G87"/>
-    </row>
-    <row r="88" spans="2:7">
+      <c r="H87"/>
+    </row>
+    <row r="88" spans="2:8">
       <c r="B88"/>
       <c r="C88"/>
       <c r="D88"/>
       <c r="E88"/>
       <c r="F88"/>
       <c r="G88"/>
-    </row>
-    <row r="89" spans="2:7">
+      <c r="H88"/>
+    </row>
+    <row r="89" spans="2:8">
       <c r="B89"/>
       <c r="C89"/>
       <c r="D89"/>
       <c r="E89"/>
       <c r="F89"/>
       <c r="G89"/>
-    </row>
-    <row r="90" spans="2:7">
+      <c r="H89"/>
+    </row>
+    <row r="90" spans="2:8">
       <c r="B90"/>
       <c r="C90"/>
       <c r="D90"/>
       <c r="E90"/>
       <c r="F90"/>
       <c r="G90"/>
-    </row>
-    <row r="91" spans="2:7">
+      <c r="H90"/>
+    </row>
+    <row r="91" spans="2:8">
       <c r="B91"/>
       <c r="C91"/>
       <c r="D91"/>
       <c r="E91"/>
       <c r="F91"/>
       <c r="G91"/>
-    </row>
-    <row r="92" spans="2:7">
+      <c r="H91"/>
+    </row>
+    <row r="92" spans="2:8">
       <c r="B92"/>
       <c r="C92"/>
       <c r="D92"/>
       <c r="E92"/>
       <c r="F92"/>
       <c r="G92"/>
-    </row>
-    <row r="93" spans="2:7">
+      <c r="H92"/>
+    </row>
+    <row r="93" spans="2:8">
       <c r="B93"/>
       <c r="C93"/>
       <c r="D93"/>
       <c r="E93"/>
       <c r="F93"/>
       <c r="G93"/>
-    </row>
-    <row r="94" spans="2:7">
+      <c r="H93"/>
+    </row>
+    <row r="94" spans="2:8">
       <c r="B94"/>
       <c r="C94"/>
       <c r="D94"/>
       <c r="E94"/>
       <c r="F94"/>
       <c r="G94"/>
-    </row>
-    <row r="95" spans="2:7">
+      <c r="H94"/>
+    </row>
+    <row r="95" spans="2:8">
       <c r="B95"/>
       <c r="C95"/>
       <c r="D95"/>
       <c r="E95"/>
       <c r="F95"/>
       <c r="G95"/>
-    </row>
-    <row r="96" spans="2:7">
+      <c r="H95"/>
+    </row>
+    <row r="96" spans="2:8">
       <c r="B96"/>
       <c r="C96"/>
       <c r="D96"/>
       <c r="E96"/>
       <c r="F96"/>
       <c r="G96"/>
-    </row>
-    <row r="97" spans="2:7">
+      <c r="H96"/>
+    </row>
+    <row r="97" spans="2:8">
       <c r="B97"/>
       <c r="C97"/>
       <c r="D97"/>
       <c r="E97"/>
       <c r="F97"/>
       <c r="G97"/>
-    </row>
-    <row r="98" spans="2:7">
+      <c r="H97"/>
+    </row>
+    <row r="98" spans="2:8">
       <c r="B98"/>
       <c r="C98"/>
       <c r="D98"/>
       <c r="E98"/>
       <c r="F98"/>
       <c r="G98"/>
-    </row>
-    <row r="99" spans="2:7">
+      <c r="H98"/>
+    </row>
+    <row r="99" spans="2:8">
       <c r="B99"/>
       <c r="C99"/>
       <c r="D99"/>
       <c r="E99"/>
       <c r="F99"/>
       <c r="G99"/>
-    </row>
-    <row r="100" spans="2:7">
+      <c r="H99"/>
+    </row>
+    <row r="100" spans="2:8">
       <c r="B100"/>
       <c r="C100"/>
       <c r="D100"/>
       <c r="E100"/>
       <c r="F100"/>
       <c r="G100"/>
-    </row>
-    <row r="101" spans="2:7">
+      <c r="H100"/>
+    </row>
+    <row r="101" spans="2:8">
       <c r="B101"/>
       <c r="C101"/>
       <c r="D101"/>
       <c r="E101"/>
       <c r="F101"/>
       <c r="G101"/>
-    </row>
-    <row r="102" spans="2:7">
+      <c r="H101"/>
+    </row>
+    <row r="102" spans="2:8">
       <c r="B102"/>
       <c r="C102"/>
       <c r="D102"/>
       <c r="E102"/>
       <c r="F102"/>
       <c r="G102"/>
-    </row>
-    <row r="103" spans="2:7">
+      <c r="H102"/>
+    </row>
+    <row r="103" spans="2:8">
       <c r="B103"/>
       <c r="C103"/>
       <c r="D103"/>
       <c r="E103"/>
       <c r="F103"/>
       <c r="G103"/>
-    </row>
-    <row r="104" spans="2:7">
+      <c r="H103"/>
+    </row>
+    <row r="104" spans="2:8">
       <c r="B104"/>
       <c r="C104"/>
       <c r="D104"/>
       <c r="E104"/>
       <c r="F104"/>
       <c r="G104"/>
-    </row>
-    <row r="105" spans="2:7">
+      <c r="H104"/>
+    </row>
+    <row r="105" spans="2:8">
       <c r="B105"/>
       <c r="C105"/>
       <c r="D105"/>
       <c r="E105"/>
       <c r="F105"/>
       <c r="G105"/>
-    </row>
-    <row r="106" spans="2:7">
+      <c r="H105"/>
+    </row>
+    <row r="106" spans="2:8">
       <c r="B106"/>
       <c r="C106"/>
       <c r="D106"/>
       <c r="E106"/>
       <c r="F106"/>
       <c r="G106"/>
-    </row>
-    <row r="107" spans="2:7">
+      <c r="H106"/>
+    </row>
+    <row r="107" spans="2:8">
       <c r="B107"/>
       <c r="C107"/>
       <c r="D107"/>
       <c r="E107"/>
       <c r="F107"/>
       <c r="G107"/>
-    </row>
-    <row r="108" spans="2:7">
+      <c r="H107"/>
+    </row>
+    <row r="108" spans="2:8">
       <c r="B108"/>
       <c r="C108"/>
       <c r="D108"/>
       <c r="E108"/>
       <c r="F108"/>
       <c r="G108"/>
+      <c r="H108"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:I1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1" display="https://www.geeksforgeeks.org/problems/graph-and-vertices/1?utm_source=youtube&amp;utm_medium=collab_striver_ytdescription&amp;utm_campaign=graph-and-vertices" xr:uid="{17355DE0-6C00-48DB-BACB-E8ACE6E6C9E7}"/>
-    <hyperlink ref="D5" r:id="rId2" display="https://www.geeksforgeeks.org/problems/bfs-traversal-of-graph/1" xr:uid="{28EA351B-FBE3-4708-8F6C-9456B40C67B1}"/>
-    <hyperlink ref="D6" r:id="rId3" display="https://www.geeksforgeeks.org/problems/depth-first-traversal-for-a-graph/1" xr:uid="{4335ECAA-CEB8-48CA-8E22-097CCD827A39}"/>
-    <hyperlink ref="D7" r:id="rId4" display="https://leetcode.com/problems/number-of-provinces/submissions/1253659971/" xr:uid="{2D26AF04-925A-443B-85D0-8CEDD6D47DC6}"/>
-    <hyperlink ref="D8" r:id="rId5" display="https://leetcode.com/problems/rotting-oranges/description/" xr:uid="{46471376-652E-409C-82A8-E079D7BB19B9}"/>
-    <hyperlink ref="D9" r:id="rId6" display="https://leetcode.com/problems/flood-fill/description/" xr:uid="{8D35A4AE-0A93-45E6-99E5-6CE9A95442A9}"/>
-    <hyperlink ref="D10" r:id="rId7" display="https://leetcode.com/problems/course-schedule/description/" xr:uid="{74ABFE22-A763-44C3-AD1B-047095FB8944}"/>
-    <hyperlink ref="D11" r:id="rId8" display="https://leetcode.com/problems/course-schedule-ii/description/" xr:uid="{BEA4A1C0-724D-4147-82A5-A0BE99EBD5E1}"/>
-    <hyperlink ref="D12" r:id="rId9" display="https://leetcode.com/problems/01-matrix/" xr:uid="{6366BA1C-E0FE-447B-B1BF-C31A024E3076}"/>
-    <hyperlink ref="D13" r:id="rId10" display="https://leetcode.com/problems/surrounded-regions/description/" xr:uid="{381A60A0-282B-4DBA-B0EE-258F6E77D18F}"/>
-    <hyperlink ref="D14" r:id="rId11" display="https://leetcode.com/problems/number-of-enclaves/description/" xr:uid="{028266A5-3C9D-4C3B-BCDD-F14E6AC888E1}"/>
-    <hyperlink ref="D15" r:id="rId12" display="https://www.geeksforgeeks.org/problems/number-of-distinct-islands/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article" xr:uid="{798FDEE1-354A-4215-82A4-86F3BF668C23}"/>
-    <hyperlink ref="D16" r:id="rId13" display="https://www.geeksforgeeks.org/problems/topological-sort/1" xr:uid="{348B0082-407E-4F2F-8E32-4FAFD22BA730}"/>
-    <hyperlink ref="D17" r:id="rId14" display="https://www.geeksforgeeks.org/problems/topological-sort/1?utm_source=youtube&amp;utm_medium=collab_striver_ytdescription&amp;utm_campaign=topological-sort" xr:uid="{6463A95A-A227-4E34-99B0-959C20F16A52}"/>
-    <hyperlink ref="D18" r:id="rId15" display="https://www.geeksforgeeks.org/problems/detect-cycle-in-a-directed-graph/1" xr:uid="{B47745D1-8041-403C-9E52-D33B17690EB2}"/>
-    <hyperlink ref="D19" r:id="rId16" display="https://leetcode.com/problems/find-eventual-safe-states/" xr:uid="{8B68E585-A98B-4F6B-A780-01ABADBE56DE}"/>
-    <hyperlink ref="D20" r:id="rId17" display="https://www.geeksforgeeks.org/problems/alien-dictionary/1" xr:uid="{F8AB8BE8-2DBA-4EC8-BF3D-EE6088A45415}"/>
-    <hyperlink ref="D25" r:id="rId18" display="https://www.geeksforgeeks.org/problems/shortest-path-in-undirected-graph-having-unit-distance/1?utm_source=youtube&amp;utm_medium=collab_striver_ytdescription&amp;utm_campaign=shortest-path-in-undirected-graph-having-unit-distance" xr:uid="{8C8DC86A-FDC3-4B8B-BA0B-4F306DAAD809}"/>
-    <hyperlink ref="D22" r:id="rId19" display="https://leetcode.com/problems/is-graph-bipartite/description/" xr:uid="{6A31382A-7A64-413C-8772-C7138054C402}"/>
-    <hyperlink ref="D26" r:id="rId20" display="https://www.geeksforgeeks.org/problems/shortest-path-in-undirected-graph/1?utm_source=youtube&amp;utm_medium=collab_striver_ytdescription&amp;utm_campaign=shortest-path-in-undirected-graph" xr:uid="{2E2B41E8-1B25-4055-B590-DECD1358F84B}"/>
-    <hyperlink ref="D27" r:id="rId21" display="https://www.geeksforgeeks.org/problems/implementing-dijkstra-set-1-adjacency-matrix/1" xr:uid="{55F4402A-4A28-467E-AFF1-52F753046B6C}"/>
-    <hyperlink ref="D28" r:id="rId22" display="https://leetcode.com/problems/shortest-path-in-binary-matrix/description/" xr:uid="{2EA1DE6D-D98C-405D-B77B-B817A426A8F3}"/>
-    <hyperlink ref="D29" r:id="rId23" display="https://leetcode.com/problems/path-with-minimum-effort/description/" xr:uid="{80B1D9FD-A236-4AE4-A862-8A606642B1B2}"/>
+    <hyperlink ref="E4" r:id="rId1" display="https://www.geeksforgeeks.org/problems/graph-and-vertices/1?utm_source=youtube&amp;utm_medium=collab_striver_ytdescription&amp;utm_campaign=graph-and-vertices" xr:uid="{17355DE0-6C00-48DB-BACB-E8ACE6E6C9E7}"/>
+    <hyperlink ref="E5" r:id="rId2" display="https://www.geeksforgeeks.org/problems/bfs-traversal-of-graph/1" xr:uid="{28EA351B-FBE3-4708-8F6C-9456B40C67B1}"/>
+    <hyperlink ref="E6" r:id="rId3" display="https://www.geeksforgeeks.org/problems/depth-first-traversal-for-a-graph/1" xr:uid="{4335ECAA-CEB8-48CA-8E22-097CCD827A39}"/>
+    <hyperlink ref="E7" r:id="rId4" display="https://leetcode.com/problems/number-of-provinces/submissions/1253659971/" xr:uid="{2D26AF04-925A-443B-85D0-8CEDD6D47DC6}"/>
+    <hyperlink ref="E8" r:id="rId5" display="https://leetcode.com/problems/rotting-oranges/description/" xr:uid="{46471376-652E-409C-82A8-E079D7BB19B9}"/>
+    <hyperlink ref="E9" r:id="rId6" display="https://leetcode.com/problems/flood-fill/description/" xr:uid="{8D35A4AE-0A93-45E6-99E5-6CE9A95442A9}"/>
+    <hyperlink ref="E10" r:id="rId7" display="https://leetcode.com/problems/course-schedule/description/" xr:uid="{74ABFE22-A763-44C3-AD1B-047095FB8944}"/>
+    <hyperlink ref="E11" r:id="rId8" display="https://leetcode.com/problems/course-schedule-ii/description/" xr:uid="{BEA4A1C0-724D-4147-82A5-A0BE99EBD5E1}"/>
+    <hyperlink ref="E12" r:id="rId9" display="https://leetcode.com/problems/01-matrix/" xr:uid="{6366BA1C-E0FE-447B-B1BF-C31A024E3076}"/>
+    <hyperlink ref="E13" r:id="rId10" display="https://leetcode.com/problems/surrounded-regions/description/" xr:uid="{381A60A0-282B-4DBA-B0EE-258F6E77D18F}"/>
+    <hyperlink ref="E14" r:id="rId11" display="https://leetcode.com/problems/number-of-enclaves/description/" xr:uid="{028266A5-3C9D-4C3B-BCDD-F14E6AC888E1}"/>
+    <hyperlink ref="E15" r:id="rId12" display="https://www.geeksforgeeks.org/problems/number-of-distinct-islands/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article" xr:uid="{798FDEE1-354A-4215-82A4-86F3BF668C23}"/>
+    <hyperlink ref="E16" r:id="rId13" display="https://www.geeksforgeeks.org/problems/topological-sort/1" xr:uid="{348B0082-407E-4F2F-8E32-4FAFD22BA730}"/>
+    <hyperlink ref="E17" r:id="rId14" display="https://www.geeksforgeeks.org/problems/topological-sort/1?utm_source=youtube&amp;utm_medium=collab_striver_ytdescription&amp;utm_campaign=topological-sort" xr:uid="{6463A95A-A227-4E34-99B0-959C20F16A52}"/>
+    <hyperlink ref="E18" r:id="rId15" display="https://www.geeksforgeeks.org/problems/detect-cycle-in-a-directed-graph/1" xr:uid="{B47745D1-8041-403C-9E52-D33B17690EB2}"/>
+    <hyperlink ref="E19" r:id="rId16" display="https://leetcode.com/problems/find-eventual-safe-states/" xr:uid="{8B68E585-A98B-4F6B-A780-01ABADBE56DE}"/>
+    <hyperlink ref="E20" r:id="rId17" display="https://www.geeksforgeeks.org/problems/alien-dictionary/1" xr:uid="{F8AB8BE8-2DBA-4EC8-BF3D-EE6088A45415}"/>
+    <hyperlink ref="E25" r:id="rId18" display="https://www.geeksforgeeks.org/problems/shortest-path-in-undirected-graph-having-unit-distance/1?utm_source=youtube&amp;utm_medium=collab_striver_ytdescription&amp;utm_campaign=shortest-path-in-undirected-graph-having-unit-distance" xr:uid="{8C8DC86A-FDC3-4B8B-BA0B-4F306DAAD809}"/>
+    <hyperlink ref="E22" r:id="rId19" display="https://leetcode.com/problems/is-graph-bipartite/description/" xr:uid="{6A31382A-7A64-413C-8772-C7138054C402}"/>
+    <hyperlink ref="E26" r:id="rId20" display="https://www.geeksforgeeks.org/problems/shortest-path-in-undirected-graph/1?utm_source=youtube&amp;utm_medium=collab_striver_ytdescription&amp;utm_campaign=shortest-path-in-undirected-graph" xr:uid="{2E2B41E8-1B25-4055-B590-DECD1358F84B}"/>
+    <hyperlink ref="E27" r:id="rId21" display="https://www.geeksforgeeks.org/problems/implementing-dijkstra-set-1-adjacency-matrix/1" xr:uid="{55F4402A-4A28-467E-AFF1-52F753046B6C}"/>
+    <hyperlink ref="E28" r:id="rId22" display="https://leetcode.com/problems/shortest-path-in-binary-matrix/description/" xr:uid="{2EA1DE6D-D98C-405D-B77B-B817A426A8F3}"/>
+    <hyperlink ref="E29" r:id="rId23" display="https://leetcode.com/problems/path-with-minimum-effort/description/" xr:uid="{80B1D9FD-A236-4AE4-A862-8A606642B1B2}"/>
+    <hyperlink ref="E30" r:id="rId24" display="https://leetcode.com/problems/cheapest-flights-within-k-stops/description/" xr:uid="{E77EECB7-C5C3-43CA-BF4B-155C449CDEE9}"/>
+    <hyperlink ref="E31" r:id="rId25" display="https://leetcode.com/problems/network-delay-time/description/" xr:uid="{3B87AC66-B8A9-4C3E-965B-BC1782376FB3}"/>
+    <hyperlink ref="E32" r:id="rId26" display="https://leetcode.com/problems/number-of-ways-to-arrive-at-destination/description/" xr:uid="{97CCC25B-8E4D-46D0-A37A-F3A93CF47235}"/>
+    <hyperlink ref="E33" r:id="rId27" display="https://www.geeksforgeeks.org/problems/minimum-multiplications-to-reach-end/1?utm_source=youtube&amp;utm_medium=collab_striver_ytdescription&amp;utm_campaign=minimum-multiplications-to-reach-end" xr:uid="{A058FB43-3306-4FD9-B073-F667107ABF04}"/>
+    <hyperlink ref="E38" r:id="rId28" display="https://www.geeksforgeeks.org/problems/minimum-spanning-tree/1" xr:uid="{52BD4289-44CB-46C0-B06E-DA9E06530155}"/>
+    <hyperlink ref="E39" r:id="rId29" display="https://www.geeksforgeeks.org/problems/minimum-spanning-tree/1" xr:uid="{53C600A2-75BE-405A-8496-CC376C75C7C2}"/>
+    <hyperlink ref="E40" r:id="rId30" display="https://takeuforward.org/data-structure/disjoint-set-union-by-rank-union-by-size-path-compression-g-46/" xr:uid="{E6303375-A725-48C1-AB13-C2708FF4BAFD}"/>
+    <hyperlink ref="E41" r:id="rId31" display="https://www.geeksforgeeks.org/problems/minimum-spanning-tree/1" xr:uid="{2628174E-D795-48FE-80AA-F094FA984B6B}"/>
+    <hyperlink ref="E42" r:id="rId32" display="https://leetcode.com/problems/number-of-operations-to-make-network-connected/description/" xr:uid="{DE6D7AC4-BFD1-4B94-9429-162C559B2670}"/>
+    <hyperlink ref="E43" r:id="rId33" display="https://leetcode.com/problems/most-stones-removed-with-same-row-or-column/" xr:uid="{BB999C07-39EB-49E4-8F60-66F1A359160C}"/>
+    <hyperlink ref="E44" r:id="rId34" display="https://leetcode.com/problems/accounts-merge/description/" xr:uid="{C313CB97-AE78-4B23-A9CA-A8D0EB5E8422}"/>
+    <hyperlink ref="E45" r:id="rId35" display="https://takeuforward.org/graph/number-of-islands-ii-online-queries-dsu-g-51/" xr:uid="{AD3F9430-6E7C-4568-AE79-609B8479BB72}"/>
+    <hyperlink ref="E46" r:id="rId36" display="https://leetcode.com/problems/making-a-large-island/description/" xr:uid="{604C4478-9E00-4401-A6DC-424D2C7219CD}"/>
+    <hyperlink ref="E47" r:id="rId37" display="https://leetcode.com/problems/swim-in-rising-water/description/" xr:uid="{000FC0FD-A1A5-426E-89E6-CBDCD2A9F540}"/>
+    <hyperlink ref="E49" r:id="rId38" display="https://leetcode.com/problems/critical-connections-in-a-network/description/" xr:uid="{716AB346-44EB-4FFA-A569-56CB33D687EA}"/>
+    <hyperlink ref="E50" r:id="rId39" display="https://www.geeksforgeeks.org/problems/articulation-point-1/1?utm_source=youtube&amp;utm_medium=collab_striver_ytdescription&amp;utm_campaign=articulation-point" xr:uid="{5E62B288-DB37-4DA6-8E2E-9E11B3D26B45}"/>
+    <hyperlink ref="E52" r:id="rId40" display="https://www.geeksforgeeks.org/problems/strongly-connected-components-kosarajus-algo/1?utm_source=youtube&amp;utm_medium=collab_striver_ytdescription&amp;utm_campaign=strongly-connected-components-kosarajus-algo" xr:uid="{EE0C2E6E-8C73-450D-846E-55AD668E2E66}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId24"/>
+  <pageSetup orientation="portrait" r:id="rId41"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9083FD8C-7ED1-4DBA-A85D-AF2678121AB5}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="15.25" customWidth="1"/>
+    <col min="4" max="4" width="56.375" customWidth="1"/>
+    <col min="5" max="5" width="72.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="25" t="s">
+        <v>483</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>481</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="B3" s="21"/>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>484</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>485</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="C11">
+        <v>9</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="C13">
+        <v>11</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="C14">
+        <v>12</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="C15">
+        <v>13</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="C16">
+        <v>14</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5">
+      <c r="C17">
+        <v>15</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5">
+      <c r="C18">
+        <v>16</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5">
+      <c r="C19">
+        <v>17</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5">
+      <c r="C20">
+        <v>18</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5">
+      <c r="C21">
+        <v>19</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5">
+      <c r="C22">
+        <v>20</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5">
+      <c r="C23">
+        <v>21</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5">
+      <c r="C24">
+        <v>22</v>
+      </c>
+      <c r="D24" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5">
+      <c r="C25">
+        <v>23</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5">
+      <c r="C26">
+        <v>24</v>
+      </c>
+      <c r="D26" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5">
+      <c r="C27">
+        <v>25</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5">
+      <c r="C28">
+        <v>26</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5">
+      <c r="C29">
+        <v>27</v>
+      </c>
+      <c r="E29" s="17" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5">
+      <c r="C30">
+        <v>28</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5">
+      <c r="C31">
+        <v>29</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="32" spans="3:5">
+      <c r="C32">
+        <v>30</v>
+      </c>
+      <c r="D32" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5">
+      <c r="C33">
+        <v>31</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5">
+      <c r="C34">
+        <v>32</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5">
+      <c r="C35">
+        <v>33</v>
+      </c>
+      <c r="D35" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5">
+      <c r="C36">
+        <v>34</v>
+      </c>
+      <c r="D36" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="37" spans="3:5">
+      <c r="C37">
+        <v>35</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>518</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1" display="https://leetcode.com/problems/minimum-area-rectangle/description/" xr:uid="{97B3CDB7-0688-487E-ADE3-9E6BF8A70B0E}"/>
+    <hyperlink ref="E4" r:id="rId2" display="https://leetcode.com/problems/minimum-area-rectangle-ii/description/" xr:uid="{75251EC4-C225-4E8A-B16B-2083E2D5C67B}"/>
+    <hyperlink ref="E5" r:id="rId3" display="https://leetcode.com/problems/shortest-path-in-a-grid-with-obstacles-elimination/description/" xr:uid="{0308007A-630B-4103-A3CA-D43C4C75D5C0}"/>
+    <hyperlink ref="E6" r:id="rId4" display="https://leetcode.com/problems/find-all-duplicates-in-an-array/description/" xr:uid="{17EDC643-D938-490E-9A2C-6C68503E3BD4}"/>
+    <hyperlink ref="E7" r:id="rId5" display="https://leetcode.com/problems/shortest-path-in-binary-matrix/description/" xr:uid="{20BD9013-776A-4E07-9932-C80FFF7FBC63}"/>
+    <hyperlink ref="E8" r:id="rId6" display="https://leetcode.com/problems/basic-calculator/description/" xr:uid="{4DAB08B6-DE03-4E59-9715-67D34F6DA5CD}"/>
+    <hyperlink ref="E9" r:id="rId7" display="https://leetcode.com/problems/basic-calculator-iv/description/" xr:uid="{4123A178-D382-49C6-A301-524BA8AEAB6C}"/>
+    <hyperlink ref="E10" r:id="rId8" display="https://leetcode.com/problems/text-justification/description/" xr:uid="{DCD62365-5BD8-4657-9EEE-20526980CABF}"/>
+    <hyperlink ref="E11" r:id="rId9" display="https://leetcode.com/problems/accounts-merge/description/" xr:uid="{E59A1A93-A058-4AF9-8BF4-CB8B919FF160}"/>
+    <hyperlink ref="E12" r:id="rId10" display="https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-tree/description/" xr:uid="{33B91044-8D7C-4193-B696-2F9DE1137A03}"/>
+    <hyperlink ref="E13" r:id="rId11" display="https://leetcode.com/problems/largest-plus-sign/description/" xr:uid="{076C181E-F15E-4366-B95D-772B000584CE}"/>
+    <hyperlink ref="E14" r:id="rId12" display="https://leetcode.com/problems/minimum-time-difference/description/" xr:uid="{E6BABE3E-C90C-4722-A2A5-5DA1CA57571E}"/>
+    <hyperlink ref="E15" r:id="rId13" display="https://leetcode.com/problems/longest-increasing-path-in-a-matrix/description/" xr:uid="{E1F9FBAB-8971-4C79-A3A2-2B1391D26D32}"/>
+    <hyperlink ref="E16" r:id="rId14" display="https://leetcode.com/problems/string-to-integer-atoi/description/" xr:uid="{3068DEEB-329C-47B7-89C5-B1D8B5CA5A50}"/>
+    <hyperlink ref="E17" r:id="rId15" display="https://leetcode.com/problems/step-by-step-directions-from-a-binary-tree-node-to-another/description/" xr:uid="{22833F2F-CB1B-4D4E-8E24-FE11F1D7C4D7}"/>
+    <hyperlink ref="E18" r:id="rId16" display="https://leetcode.com/problems/remove-all-adjacent-duplicates-in-string/description/" xr:uid="{C44F1E67-AEF3-40C1-A283-3219D1245B87}"/>
+    <hyperlink ref="E19" r:id="rId17" display="https://leetcode.com/problems/simplify-path/description/" xr:uid="{0CD7556C-302F-4917-8529-5ACF6CB36677}"/>
+    <hyperlink ref="E20" r:id="rId18" display="https://leetcode.com/problems/letter-combinations-of-a-phone-number/description/" xr:uid="{6231F1C7-A69A-4A96-8C23-565C0F085831}"/>
+    <hyperlink ref="E21" r:id="rId19" display="https://leetcode.com/problems/kth-largest-element-in-an-array/description/" xr:uid="{89EA0780-42CA-4DA8-9002-A67F6B6B1F99}"/>
+    <hyperlink ref="E22" r:id="rId20" display="https://leetcode.com/problems/number-of-islands/description/" xr:uid="{092AF5B0-5ACF-4C62-B521-633096513614}"/>
+    <hyperlink ref="E23" r:id="rId21" display="https://leetcode.com/problems/max-area-of-island/description/" xr:uid="{58B968CC-DECC-4EFD-B475-F3670FC1E84F}"/>
+    <hyperlink ref="E25" r:id="rId22" display="https://leetcode.com/problems/minimum-number-of-refueling-stops/description/" xr:uid="{8590F3C7-AE8E-47CB-816B-1B70E52E8CD0}"/>
+    <hyperlink ref="E27" r:id="rId23" display="https://leetcode.com/problems/find-median-from-data-stream/description/" xr:uid="{65286147-8308-4930-8080-344B1243243B}"/>
+    <hyperlink ref="E28" r:id="rId24" display="https://leetcode.com/problems/split-array-largest-sum/description/" xr:uid="{4B1EEE69-9467-49BE-A0DF-D182AD9EC4EB}"/>
+    <hyperlink ref="E29" r:id="rId25" display="https://leetcode.com/problems/car-pooling/description/" xr:uid="{48626C32-10AB-4A7F-B0DE-A2BEFB7A69B8}"/>
+    <hyperlink ref="E30" r:id="rId26" display="https://leetcode.com/problems/find-all-people-with-secret/description/" xr:uid="{6DFA3EFF-F6DF-4D3D-8D6E-3AC27A2E3514}"/>
+    <hyperlink ref="E31" r:id="rId27" display="https://leetcode.com/problems/evaluate-reverse-polish-notation/description/" xr:uid="{69833D93-A912-4B82-9E51-048D98B025F4}"/>
+    <hyperlink ref="E33" r:id="rId28" display="https://leetcode.com/problems/validate-binary-tree-nodes/description/" xr:uid="{5D5E4CF6-026F-46FA-B2DF-F9A5A77A6F2C}"/>
+    <hyperlink ref="E34" r:id="rId29" display="https://leetcode.com/problems/clone-graph/description/" xr:uid="{73000910-75FB-41A5-89E7-384273A86C1D}"/>
+    <hyperlink ref="E37" r:id="rId30" display="https://leetcode.com/problems/number-of-visible-people-in-a-queue/description/" xr:uid="{C5901050-E053-408E-9825-1B37436140AD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5019,4 +6017,234 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEFF8342-5904-4C8A-A244-8D861DB0689A}">
+  <dimension ref="B3:H24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="7" max="7" width="30.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:8">
+      <c r="B3" t="s">
+        <v>424</v>
+      </c>
+      <c r="C3">
+        <v>16575</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="B4" t="s">
+        <v>425</v>
+      </c>
+      <c r="C4">
+        <v>25000</v>
+      </c>
+      <c r="G4" t="s">
+        <v>437</v>
+      </c>
+      <c r="H4" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8">
+      <c r="B5" t="s">
+        <v>426</v>
+      </c>
+      <c r="C5">
+        <v>15990</v>
+      </c>
+      <c r="G5" t="s">
+        <v>438</v>
+      </c>
+      <c r="H5" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8">
+      <c r="B6" t="s">
+        <v>427</v>
+      </c>
+      <c r="C6">
+        <v>17900</v>
+      </c>
+      <c r="G6" t="s">
+        <v>439</v>
+      </c>
+      <c r="H6" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8">
+      <c r="B7" t="s">
+        <v>428</v>
+      </c>
+      <c r="C7">
+        <v>19325</v>
+      </c>
+      <c r="G7" t="s">
+        <v>440</v>
+      </c>
+      <c r="H7" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="B8" t="s">
+        <v>429</v>
+      </c>
+      <c r="C8">
+        <v>19650</v>
+      </c>
+      <c r="G8" t="s">
+        <v>441</v>
+      </c>
+      <c r="H8" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8">
+      <c r="B9" t="s">
+        <v>430</v>
+      </c>
+      <c r="C9">
+        <v>19975</v>
+      </c>
+      <c r="G9" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8">
+      <c r="B10" t="s">
+        <v>431</v>
+      </c>
+      <c r="C10">
+        <v>20250</v>
+      </c>
+      <c r="G10" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8">
+      <c r="B11" t="s">
+        <v>432</v>
+      </c>
+      <c r="C11">
+        <v>20375</v>
+      </c>
+      <c r="G11" t="s">
+        <v>442</v>
+      </c>
+      <c r="H11" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8">
+      <c r="B12" t="s">
+        <v>433</v>
+      </c>
+      <c r="C12">
+        <v>20650</v>
+      </c>
+      <c r="G12" t="s">
+        <v>443</v>
+      </c>
+      <c r="H12" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8">
+      <c r="B13" t="s">
+        <v>434</v>
+      </c>
+      <c r="C13">
+        <v>20925</v>
+      </c>
+      <c r="G13" t="s">
+        <v>444</v>
+      </c>
+      <c r="H13" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8">
+      <c r="B14" t="s">
+        <v>435</v>
+      </c>
+      <c r="C14">
+        <v>21950</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8">
+      <c r="B15" t="s">
+        <v>424</v>
+      </c>
+      <c r="C15">
+        <v>22325</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8">
+      <c r="B16" t="s">
+        <v>425</v>
+      </c>
+      <c r="C16">
+        <v>22750</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" t="s">
+        <v>426</v>
+      </c>
+      <c r="C17">
+        <v>23125</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" t="s">
+        <v>427</v>
+      </c>
+      <c r="C18">
+        <v>23500</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="B20" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3">
+      <c r="B21" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3">
+      <c r="B24" t="s">
+        <v>436</v>
+      </c>
+      <c r="C24">
+        <f>SUM(C3:C22)</f>
+        <v>330265</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="10" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding questions to Study Plan
</commit_message>
<xml_diff>
--- a/StudyPlan.xlsx
+++ b/StudyPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rammi\Documents\Ram\Learning\ram-err404\Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF97A621-AF09-44F4-B987-1DBEA15DB3FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E506EAD-C9C4-4C90-A6D9-BD51C8554A57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{DBD4FF11-46FB-5146-978E-3349D45A0734}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="579">
   <si>
     <t>Programming Topics</t>
   </si>
@@ -1601,6 +1601,186 @@
   </si>
   <si>
     <t>Number of Visible People in a Queue - LeetCode</t>
+  </si>
+  <si>
+    <t>Nested List Weight Sum</t>
+  </si>
+  <si>
+    <t>Race Car - LeetCode</t>
+  </si>
+  <si>
+    <t>Basic Calculator 3</t>
+  </si>
+  <si>
+    <t>Design In-Memory File System</t>
+  </si>
+  <si>
+    <t>Invert Binary Tree - LeetCode</t>
+  </si>
+  <si>
+    <t>Maximum Points You Can Obtain from Cards - LeetCode</t>
+  </si>
+  <si>
+    <t>Stock Price Fluctuation - LeetCode</t>
+  </si>
+  <si>
+    <t>Time Needed to Inform All Employees - LeetCode</t>
+  </si>
+  <si>
+    <t>Maximum Split of Positive Even Integers - LeetCode</t>
+  </si>
+  <si>
+    <t>Count Words Obtained After Adding a Letter - LeetCode</t>
+  </si>
+  <si>
+    <t>Find Duplicate Subtrees - LeetCode</t>
+  </si>
+  <si>
+    <t>Product of the Last K Numbers - LeetCode</t>
+  </si>
+  <si>
+    <t>shortest-path-to-get-food</t>
+  </si>
+  <si>
+    <t>Word Break II - LeetCode</t>
+  </si>
+  <si>
+    <t>Word Ladder - LeetCode</t>
+  </si>
+  <si>
+    <t>Word Ladder II - LeetCode</t>
+  </si>
+  <si>
+    <t>Follow Up</t>
+  </si>
+  <si>
+    <t>Random Pick with Weight - LeetCode</t>
+  </si>
+  <si>
+    <t>amount-of-new-area-painted-each-day</t>
+  </si>
+  <si>
+    <t>closest-binary-search-tree-value-ii</t>
+  </si>
+  <si>
+    <t>The Number of Weak Characters in the Game - LeetCode</t>
+  </si>
+  <si>
+    <t>First Missing Positive - LeetCode</t>
+  </si>
+  <si>
+    <t>Subtree of Another Tree - LeetCode</t>
+  </si>
+  <si>
+    <t>Container With Most Water - LeetCode</t>
+  </si>
+  <si>
+    <t>Best Time to Buy and Sell Stock - LeetCode</t>
+  </si>
+  <si>
+    <t>Minimum Window Substring - LeetCode</t>
+  </si>
+  <si>
+    <t>Delete Nodes And Return Forest - LeetCode</t>
+  </si>
+  <si>
+    <t>Random Pick Index - LeetCode</t>
+  </si>
+  <si>
+    <t>strobogrammatic-number</t>
+  </si>
+  <si>
+    <t>largest-bst-subtree</t>
+  </si>
+  <si>
+    <t>design-hit-counter</t>
+  </si>
+  <si>
+    <t>shortest-distance-from-all-buildings</t>
+  </si>
+  <si>
+    <t>Find All Possible Recipes from Given Supplies - LeetCode</t>
+  </si>
+  <si>
+    <t>Max Consecutive Ones III - LeetCode</t>
+  </si>
+  <si>
+    <t>Sum of Prefix Scores of Strings - LeetCode</t>
+  </si>
+  <si>
+    <t>Exclusive Time of Functions - LeetCode</t>
+  </si>
+  <si>
+    <t>My Calendar I - LeetCode</t>
+  </si>
+  <si>
+    <t>Expression Add Operators - LeetCode</t>
+  </si>
+  <si>
+    <t>add-bold-tag-in-string</t>
+  </si>
+  <si>
+    <t>Range Module - LeetCode</t>
+  </si>
+  <si>
+    <t>Detect Squares - LeetCode</t>
+  </si>
+  <si>
+    <t>shortest-way-to-form-string</t>
+  </si>
+  <si>
+    <t>Detonate the Maximum Bombs - LeetCode</t>
+  </si>
+  <si>
+    <t>Count of Smaller Numbers After Self - LeetCode</t>
+  </si>
+  <si>
+    <t>longest-line-of-consecutive-one-in-matrix</t>
+  </si>
+  <si>
+    <t>Count Unique Characters of All Substrings of a Given String - LeetCode</t>
+  </si>
+  <si>
+    <t>All Paths From Source to Target - LeetCode</t>
+  </si>
+  <si>
+    <t>the-earliest-moment-when-everyone-become-friends</t>
+  </si>
+  <si>
+    <t>Implement Trie (Prefix Tree) - LeetCode</t>
+  </si>
+  <si>
+    <t>Meeting Rooms III - LeetCode</t>
+  </si>
+  <si>
+    <t>parallel-courses</t>
+  </si>
+  <si>
+    <t>Maximum Subarray Sum with One Deletion - LeetCode</t>
+  </si>
+  <si>
+    <t>alien-dictionary</t>
+  </si>
+  <si>
+    <t>Longest Consecutive Sequence - LeetCode</t>
+  </si>
+  <si>
+    <t>Top K Frequent Words - LeetCode</t>
+  </si>
+  <si>
+    <t>Count Nodes Equal to Average of Subtree - LeetCode</t>
+  </si>
+  <si>
+    <t>find-distance-in-a-binary-tree</t>
+  </si>
+  <si>
+    <t>Trapping Rain Water - LeetCode</t>
+  </si>
+  <si>
+    <t>Insert Interval - LeetCode</t>
+  </si>
+  <si>
+    <t>Find Number of Coins to Place in Tree Nodes - LeetCode</t>
   </si>
 </sst>
 </file>
@@ -1826,7 +2006,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1871,6 +2051,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5640,21 +5821,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9083FD8C-7ED1-4DBA-A85D-AF2678121AB5}">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:G96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A96" sqref="A96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="15.25" customWidth="1"/>
-    <col min="4" max="4" width="56.375" customWidth="1"/>
-    <col min="5" max="5" width="72.375" customWidth="1"/>
+    <col min="2" max="2" width="11.875" customWidth="1"/>
+    <col min="4" max="4" width="53.375" customWidth="1"/>
+    <col min="5" max="5" width="62.25" customWidth="1"/>
+    <col min="6" max="6" width="31.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="25" t="s">
         <v>483</v>
       </c>
@@ -5663,7 +5845,7 @@
       <c r="D1" s="25"/>
       <c r="E1" s="25"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" s="22" t="s">
         <v>83</v>
       </c>
@@ -5679,8 +5861,11 @@
       <c r="E2" s="22" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="26" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="B3" s="21"/>
       <c r="C3">
         <v>1</v>
@@ -5692,7 +5877,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="C4">
         <v>2</v>
       </c>
@@ -5703,7 +5888,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="C5">
         <v>3</v>
       </c>
@@ -5711,7 +5896,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="C6">
         <v>4</v>
       </c>
@@ -5719,7 +5904,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="C7">
         <v>5</v>
       </c>
@@ -5727,7 +5912,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="C8">
         <v>6</v>
       </c>
@@ -5735,7 +5920,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:6">
       <c r="C9">
         <v>7</v>
       </c>
@@ -5743,7 +5928,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:6">
       <c r="C10">
         <v>8</v>
       </c>
@@ -5751,7 +5936,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:6">
       <c r="C11">
         <v>9</v>
       </c>
@@ -5759,7 +5944,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:6">
       <c r="C12">
         <v>10</v>
       </c>
@@ -5767,7 +5952,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:6">
       <c r="C13">
         <v>11</v>
       </c>
@@ -5775,7 +5960,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:6">
       <c r="C14">
         <v>12</v>
       </c>
@@ -5783,7 +5968,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:6">
       <c r="C15">
         <v>13</v>
       </c>
@@ -5791,7 +5976,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:6">
       <c r="C16">
         <v>14</v>
       </c>
@@ -5965,6 +6150,493 @@
       </c>
       <c r="E37" s="17" t="s">
         <v>518</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5">
+      <c r="C38">
+        <v>36</v>
+      </c>
+      <c r="D38" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="39" spans="3:5">
+      <c r="C39">
+        <v>37</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="40" spans="3:5">
+      <c r="C40">
+        <v>38</v>
+      </c>
+      <c r="D40" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="41" spans="3:5">
+      <c r="C41">
+        <v>39</v>
+      </c>
+      <c r="D41" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="42" spans="3:5">
+      <c r="C42">
+        <v>40</v>
+      </c>
+      <c r="E42" s="17" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="43" spans="3:5">
+      <c r="C43">
+        <v>41</v>
+      </c>
+      <c r="E43" s="17" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="44" spans="3:5">
+      <c r="C44">
+        <v>42</v>
+      </c>
+      <c r="E44" s="17" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="45" spans="3:5">
+      <c r="C45">
+        <v>43</v>
+      </c>
+      <c r="E45" s="17" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="46" spans="3:5">
+      <c r="C46">
+        <v>44</v>
+      </c>
+      <c r="E46" s="17" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="47" spans="3:5">
+      <c r="C47">
+        <v>45</v>
+      </c>
+      <c r="E47" s="17" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="48" spans="3:5">
+      <c r="C48">
+        <v>46</v>
+      </c>
+      <c r="E48" s="17" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="49" spans="3:6">
+      <c r="C49">
+        <v>47</v>
+      </c>
+      <c r="E49" s="17" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6">
+      <c r="C50">
+        <v>48</v>
+      </c>
+      <c r="D50" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="51" spans="3:6">
+      <c r="C51">
+        <v>49</v>
+      </c>
+      <c r="E51" s="17" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="52" spans="3:6">
+      <c r="C52">
+        <v>50</v>
+      </c>
+      <c r="E52" s="17" t="s">
+        <v>533</v>
+      </c>
+      <c r="F52" s="17" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="53" spans="3:6">
+      <c r="C53">
+        <v>51</v>
+      </c>
+      <c r="E53" s="17" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="54" spans="3:6">
+      <c r="C54">
+        <v>52</v>
+      </c>
+      <c r="D54" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="55" spans="3:6">
+      <c r="C55">
+        <v>53</v>
+      </c>
+      <c r="D55" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="56" spans="3:6">
+      <c r="C56">
+        <v>54</v>
+      </c>
+      <c r="E56" s="17" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="57" spans="3:6">
+      <c r="C57">
+        <v>55</v>
+      </c>
+      <c r="E57" s="17" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="58" spans="3:6">
+      <c r="C58">
+        <v>56</v>
+      </c>
+      <c r="E58" s="17" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="59" spans="3:6">
+      <c r="C59">
+        <v>57</v>
+      </c>
+      <c r="E59" s="17" t="s">
+        <v>387</v>
+      </c>
+      <c r="F59" s="17" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="60" spans="3:6">
+      <c r="C60">
+        <v>58</v>
+      </c>
+      <c r="E60" s="17" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="61" spans="3:6">
+      <c r="C61">
+        <v>59</v>
+      </c>
+      <c r="E61" s="17" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="62" spans="3:6">
+      <c r="C62">
+        <v>60</v>
+      </c>
+      <c r="E62" s="17" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="63" spans="3:6">
+      <c r="C63">
+        <v>61</v>
+      </c>
+      <c r="E63" s="17" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="64" spans="3:6">
+      <c r="C64">
+        <v>62</v>
+      </c>
+      <c r="E64" s="17" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="65" spans="3:7">
+      <c r="C65">
+        <v>63</v>
+      </c>
+      <c r="E65" s="17" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="66" spans="3:7">
+      <c r="C66">
+        <v>64</v>
+      </c>
+      <c r="D66" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="67" spans="3:7">
+      <c r="C67">
+        <v>65</v>
+      </c>
+      <c r="D67" t="s">
+        <v>548</v>
+      </c>
+      <c r="G67" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="68" spans="3:7">
+      <c r="C68">
+        <v>66</v>
+      </c>
+      <c r="D68" t="s">
+        <v>549</v>
+      </c>
+      <c r="G68" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="69" spans="3:7">
+      <c r="C69">
+        <v>67</v>
+      </c>
+      <c r="D69" t="s">
+        <v>550</v>
+      </c>
+      <c r="G69" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70" spans="3:7">
+      <c r="C70">
+        <v>68</v>
+      </c>
+      <c r="E70" s="17" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="71" spans="3:7">
+      <c r="C71">
+        <v>69</v>
+      </c>
+      <c r="E71" s="17" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="72" spans="3:7">
+      <c r="C72">
+        <v>70</v>
+      </c>
+      <c r="E72" s="17" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="73" spans="3:7">
+      <c r="C73">
+        <v>71</v>
+      </c>
+      <c r="E73" s="17" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="74" spans="3:7">
+      <c r="C74">
+        <v>72</v>
+      </c>
+      <c r="E74" s="17" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="75" spans="3:7">
+      <c r="C75">
+        <v>73</v>
+      </c>
+      <c r="D75" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="76" spans="3:7">
+      <c r="C76">
+        <v>74</v>
+      </c>
+      <c r="E76" s="17" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="77" spans="3:7">
+      <c r="C77">
+        <v>75</v>
+      </c>
+      <c r="E77" s="17" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="78" spans="3:7">
+      <c r="C78">
+        <v>76</v>
+      </c>
+      <c r="D78" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="79" spans="3:7">
+      <c r="C79">
+        <v>77</v>
+      </c>
+      <c r="E79" s="17" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="80" spans="3:7">
+      <c r="C80">
+        <v>78</v>
+      </c>
+      <c r="E80" s="17" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="81" spans="3:5">
+      <c r="C81">
+        <v>79</v>
+      </c>
+      <c r="D81" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="82" spans="3:5">
+      <c r="C82">
+        <v>80</v>
+      </c>
+      <c r="E82" s="17" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="83" spans="3:5">
+      <c r="C83">
+        <v>81</v>
+      </c>
+      <c r="E83" s="17" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="84" spans="3:5">
+      <c r="C84">
+        <v>82</v>
+      </c>
+      <c r="D84" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="85" spans="3:5">
+      <c r="C85">
+        <v>83</v>
+      </c>
+      <c r="E85" s="17" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="86" spans="3:5">
+      <c r="C86">
+        <v>84</v>
+      </c>
+      <c r="E86" s="17" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="87" spans="3:5">
+      <c r="C87">
+        <v>85</v>
+      </c>
+      <c r="D87" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="88" spans="3:5">
+      <c r="C88">
+        <v>86</v>
+      </c>
+      <c r="E88" s="17" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="89" spans="3:5">
+      <c r="C89">
+        <v>87</v>
+      </c>
+      <c r="D89" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="90" spans="3:5">
+      <c r="C90">
+        <v>88</v>
+      </c>
+      <c r="E90" s="17" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="91" spans="3:5">
+      <c r="C91">
+        <v>89</v>
+      </c>
+      <c r="E91" s="17" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="92" spans="3:5">
+      <c r="C92">
+        <v>90</v>
+      </c>
+      <c r="E92" s="17" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="93" spans="3:5">
+      <c r="C93">
+        <v>91</v>
+      </c>
+      <c r="D93" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="94" spans="3:5">
+      <c r="C94">
+        <v>92</v>
+      </c>
+      <c r="E94" s="17" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="95" spans="3:5">
+      <c r="C95">
+        <v>93</v>
+      </c>
+      <c r="E95" s="17" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="96" spans="3:5">
+      <c r="C96">
+        <v>94</v>
+      </c>
+      <c r="E96" s="17" t="s">
+        <v>578</v>
       </c>
     </row>
   </sheetData>
@@ -6002,6 +6674,50 @@
     <hyperlink ref="E33" r:id="rId28" display="https://leetcode.com/problems/validate-binary-tree-nodes/description/" xr:uid="{5D5E4CF6-026F-46FA-B2DF-F9A5A77A6F2C}"/>
     <hyperlink ref="E34" r:id="rId29" display="https://leetcode.com/problems/clone-graph/description/" xr:uid="{73000910-75FB-41A5-89E7-384273A86C1D}"/>
     <hyperlink ref="E37" r:id="rId30" display="https://leetcode.com/problems/number-of-visible-people-in-a-queue/description/" xr:uid="{C5901050-E053-408E-9825-1B37436140AD}"/>
+    <hyperlink ref="E39" r:id="rId31" display="https://leetcode.com/problems/race-car/description/" xr:uid="{F34BD829-0806-48D6-8E94-36DAC28C05B2}"/>
+    <hyperlink ref="E42" r:id="rId32" display="https://leetcode.com/problems/invert-binary-tree/description/" xr:uid="{FFE3BF16-BD35-4A18-B8ED-D5F6A3D984F5}"/>
+    <hyperlink ref="E43" r:id="rId33" display="https://leetcode.com/problems/maximum-points-you-can-obtain-from-cards/description/" xr:uid="{C695D906-3D3A-4D94-B844-BAC1499909CF}"/>
+    <hyperlink ref="E44" r:id="rId34" display="https://leetcode.com/problems/stock-price-fluctuation/description/" xr:uid="{CEB5E06E-A83C-4CE9-88BF-E41EB4B47AE6}"/>
+    <hyperlink ref="E45" r:id="rId35" display="https://leetcode.com/problems/time-needed-to-inform-all-employees/description/" xr:uid="{54CAF010-93C5-4B50-9CD9-FC52AA395EFD}"/>
+    <hyperlink ref="E46" r:id="rId36" display="https://leetcode.com/problems/maximum-split-of-positive-even-integers/description/" xr:uid="{8023B33A-C461-4129-8B23-38A0F3BDB249}"/>
+    <hyperlink ref="E47" r:id="rId37" display="https://leetcode.com/problems/count-words-obtained-after-adding-a-letter/description/" xr:uid="{6B128D41-7D0F-4578-918E-846978443C2D}"/>
+    <hyperlink ref="E48" r:id="rId38" display="https://leetcode.com/problems/find-duplicate-subtrees/description/" xr:uid="{CE403545-6F24-4AE0-BBA2-0688D496DA79}"/>
+    <hyperlink ref="E49" r:id="rId39" display="https://leetcode.com/problems/product-of-the-last-k-numbers/description/" xr:uid="{A457C4D2-E78B-430E-8105-CE163D0AA41E}"/>
+    <hyperlink ref="E51" r:id="rId40" display="https://leetcode.com/problems/word-break-ii/description/" xr:uid="{D8F3DEE7-52D0-425B-B1F2-E22D420A808E}"/>
+    <hyperlink ref="E52" r:id="rId41" display="https://leetcode.com/problems/word-ladder/description/" xr:uid="{CA15EF06-DA87-4008-AB32-ACCB219EBDED}"/>
+    <hyperlink ref="F52" r:id="rId42" display="https://leetcode.com/problems/word-ladder-ii/description/" xr:uid="{DF2DE128-AF49-47A8-89E3-957099AEB7F9}"/>
+    <hyperlink ref="E53" r:id="rId43" display="https://leetcode.com/problems/random-pick-with-weight/description/" xr:uid="{2A1A5561-9E90-4B53-BF28-0CE37E897575}"/>
+    <hyperlink ref="E56" r:id="rId44" display="https://leetcode.com/problems/the-number-of-weak-characters-in-the-game/description/" xr:uid="{FC7AE504-5C4E-4D18-9BD7-D2F4AEADAA8D}"/>
+    <hyperlink ref="E57" r:id="rId45" display="https://leetcode.com/problems/first-missing-positive/description/" xr:uid="{D49343EB-3F61-4B22-AAC1-C5D59BCF6372}"/>
+    <hyperlink ref="E58" r:id="rId46" display="https://leetcode.com/problems/subtree-of-another-tree/description/" xr:uid="{A4598857-829B-4813-A9BD-16C86FED9729}"/>
+    <hyperlink ref="E59" r:id="rId47" display="https://leetcode.com/problems/course-schedule/description/" xr:uid="{5B4AF7EF-A67C-453D-842F-6A45CDC40BEA}"/>
+    <hyperlink ref="F59" r:id="rId48" display="https://leetcode.com/problems/course-schedule-ii/description/" xr:uid="{E8E2442C-203D-43C6-91DF-0F6BFFD1B82A}"/>
+    <hyperlink ref="E60" r:id="rId49" display="https://leetcode.com/problems/container-with-most-water/description/" xr:uid="{DD7468F9-8202-4357-8F67-E25A3F1F475A}"/>
+    <hyperlink ref="E61" r:id="rId50" display="https://leetcode.com/problems/best-time-to-buy-and-sell-stock/description/" xr:uid="{F96333BD-57F3-4B59-A45B-8E2B90D1DA31}"/>
+    <hyperlink ref="E62" r:id="rId51" display="https://leetcode.com/problems/minimum-window-substring/description/" xr:uid="{721C4F62-099D-430A-9D00-C83588380485}"/>
+    <hyperlink ref="E63" r:id="rId52" display="https://leetcode.com/problems/delete-nodes-and-return-forest/description/" xr:uid="{BF7A8635-E1DE-4044-911C-2972ED4835F9}"/>
+    <hyperlink ref="E64" r:id="rId53" display="https://leetcode.com/problems/random-pick-index/description/" xr:uid="{500A76D1-930D-47A5-8EDB-92F3BD624B44}"/>
+    <hyperlink ref="E70" r:id="rId54" display="https://leetcode.com/problems/find-all-possible-recipes-from-given-supplies/description/" xr:uid="{57C1F90F-C049-4C1A-AC6F-1389A59F118A}"/>
+    <hyperlink ref="E71" r:id="rId55" display="https://leetcode.com/problems/max-consecutive-ones-iii/description/" xr:uid="{4BEAA75F-642A-4975-BA2F-3BCEB70B7EB0}"/>
+    <hyperlink ref="E72" r:id="rId56" display="https://leetcode.com/problems/sum-of-prefix-scores-of-strings/description/" xr:uid="{5082BE44-A416-47C9-BFD3-576CBA72B93F}"/>
+    <hyperlink ref="E73" r:id="rId57" display="https://leetcode.com/problems/exclusive-time-of-functions/description/" xr:uid="{F88FB723-8FDE-4892-B814-5F74EE0964D7}"/>
+    <hyperlink ref="E74" r:id="rId58" display="https://leetcode.com/problems/my-calendar-i/description/" xr:uid="{05187863-277C-490E-8112-BB27E8BDA32B}"/>
+    <hyperlink ref="E65" r:id="rId59" display="https://leetcode.com/problems/expression-add-operators/description/" xr:uid="{AC3435EE-DE8E-444B-863D-06DE42B90A33}"/>
+    <hyperlink ref="E76" r:id="rId60" display="https://leetcode.com/problems/range-module/description/" xr:uid="{6B32F7D1-0854-478C-9BDB-464BA57713A7}"/>
+    <hyperlink ref="E77" r:id="rId61" display="https://leetcode.com/problems/detect-squares/description/" xr:uid="{5F533695-934D-49A8-8540-3815925040B7}"/>
+    <hyperlink ref="E79" r:id="rId62" display="https://leetcode.com/problems/detonate-the-maximum-bombs/description/" xr:uid="{D1DA20E3-84F6-4A80-AD20-CED7A1BB8EF0}"/>
+    <hyperlink ref="E80" r:id="rId63" display="https://leetcode.com/problems/count-of-smaller-numbers-after-self/description/" xr:uid="{C0F38841-8238-4B7F-8903-AABA087C8C45}"/>
+    <hyperlink ref="E82" r:id="rId64" display="https://leetcode.com/problems/count-unique-characters-of-all-substrings-of-a-given-string/description/" xr:uid="{0D5F0E48-7F42-4F57-A7EE-D320FF5F00F1}"/>
+    <hyperlink ref="E83" r:id="rId65" display="https://leetcode.com/problems/all-paths-from-source-to-target/description/" xr:uid="{F0A7DDD5-6713-4F7E-A57D-58BA2D478C48}"/>
+    <hyperlink ref="E85" r:id="rId66" display="https://leetcode.com/problems/implement-trie-prefix-tree/description/" xr:uid="{2291E80F-6C79-4EF7-A9B1-DA1EE83A9867}"/>
+    <hyperlink ref="E86" r:id="rId67" display="https://leetcode.com/problems/meeting-rooms-iii/description/" xr:uid="{710FEEDA-1D4D-41CF-8B31-85021F0D68E6}"/>
+    <hyperlink ref="E88" r:id="rId68" display="https://leetcode.com/problems/maximum-subarray-sum-with-one-deletion/description/" xr:uid="{21D62DA6-9B0C-4481-9D69-6CC4AFAAE5C5}"/>
+    <hyperlink ref="E90" r:id="rId69" display="https://leetcode.com/problems/longest-consecutive-sequence/description/" xr:uid="{7CCDB3DD-B0E2-492E-8CCE-7EB1A145F0D9}"/>
+    <hyperlink ref="E91" r:id="rId70" display="https://leetcode.com/problems/top-k-frequent-words/description/" xr:uid="{AA26BE3A-78D2-4421-B48C-08AA2DD3242E}"/>
+    <hyperlink ref="E92" r:id="rId71" display="https://leetcode.com/problems/count-nodes-equal-to-average-of-subtree/description/" xr:uid="{4FCCE66C-9F48-42C7-BB54-0472265ABF28}"/>
+    <hyperlink ref="E94" r:id="rId72" display="https://leetcode.com/problems/trapping-rain-water/description/" xr:uid="{DDBF8DCB-5E56-47E8-B326-24E7CD0CFB48}"/>
+    <hyperlink ref="E95" r:id="rId73" display="https://leetcode.com/problems/insert-interval/description/" xr:uid="{A1FD679B-8A7B-4E73-818E-975FD8D978E0}"/>
+    <hyperlink ref="E96" r:id="rId74" display="https://leetcode.com/problems/find-number-of-coins-to-place-in-tree-nodes/description/" xr:uid="{FCC8012D-1143-4C41-BD7A-1F1166D520ED}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>